<commit_message>
Refactor file paths and update working directory in Unsupervised_learning.R
</commit_message>
<xml_diff>
--- a/3.Applied-Supervised-Learning-Groupwork/trained_ML_models.xlsx
+++ b/3.Applied-Supervised-Learning-Groupwork/trained_ML_models.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -392,7 +392,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_4_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_AllModels_4_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B2">
@@ -411,7 +411,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_6_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_AllModels_6_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B3">
@@ -430,26 +430,26 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>StackedEnsemble_Best1000_1_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_Best1000_1_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B4">
-        <v>41463.9707910636</v>
+        <v>41454.8147379177</v>
       </c>
       <c r="C4">
-        <v>1719260873.76218</v>
+        <v>1718501664.95508</v>
       </c>
       <c r="D4">
-        <v>23296.0625709969</v>
+        <v>23294.3303148232</v>
       </c>
       <c r="F4">
-        <v>1719260873.76218</v>
+        <v>1718501664.95508</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_3_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_AllModels_3_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B5">
@@ -468,7 +468,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_2_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_AllModels_2_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B6">
@@ -487,7 +487,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_1_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_AllModels_1_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B7">
@@ -506,7 +506,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GBM_2_AutoML_2_20240525_22650</t>
+          <t>GBM_2_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B8">
@@ -525,7 +525,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_2_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_BestOfFamily_2_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B9">
@@ -544,64 +544,64 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_4_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_BestOfFamily_4_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B10">
-        <v>42046.8449644986</v>
+        <v>42046.6137318345</v>
       </c>
       <c r="C10">
-        <v>1767937171.46858</v>
+        <v>1767917726.31409</v>
       </c>
       <c r="D10">
-        <v>23824.2001977475</v>
+        <v>23824.0538579689</v>
       </c>
       <c r="F10">
-        <v>1767937171.46858</v>
+        <v>1767917726.31409</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_3_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_BestOfFamily_3_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B11">
-        <v>42047.3214395534</v>
+        <v>42049.0451578926</v>
       </c>
       <c r="C11">
-        <v>1767977240.24113</v>
+        <v>1768122198.69049</v>
       </c>
       <c r="D11">
-        <v>23821.6206375258</v>
+        <v>23822.1606639521</v>
       </c>
       <c r="F11">
-        <v>1767977240.24113</v>
+        <v>1768122198.69049</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_6_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_BestOfFamily_6_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B12">
-        <v>42081.4533153027</v>
+        <v>42076.909972133</v>
       </c>
       <c r="C12">
-        <v>1770848713.128</v>
+        <v>1770466352.80299</v>
       </c>
       <c r="D12">
-        <v>23850.7965479591</v>
+        <v>23846.2304531303</v>
       </c>
       <c r="F12">
-        <v>1770848713.128</v>
+        <v>1770466352.80299</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_16</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_16</t>
         </is>
       </c>
       <c r="B13">
@@ -620,7 +620,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_2</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_2</t>
         </is>
       </c>
       <c r="B14">
@@ -639,7 +639,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GBM_3_AutoML_2_20240525_22650</t>
+          <t>GBM_3_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B15">
@@ -658,7 +658,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_1</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_1</t>
         </is>
       </c>
       <c r="B16">
@@ -677,48 +677,48 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_5_AutoML_2_20240525_22650</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_20</t>
         </is>
       </c>
       <c r="B17">
-        <v>42207.622879947</v>
+        <v>42304.0587258997</v>
       </c>
       <c r="C17">
-        <v>1781483429.17582</v>
+        <v>1789633384.68437</v>
       </c>
       <c r="D17">
-        <v>23439.8676037476</v>
-      </c>
-      <c r="E17">
-        <v>3.00500739964509</v>
+        <v>24456.622863756</v>
       </c>
       <c r="F17">
-        <v>1781483429.17582</v>
+        <v>1789633384.68437</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_20</t>
+          <t>StackedEnsemble_AllModels_5_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B18">
-        <v>42304.0587258997</v>
+        <v>42304.9562902227</v>
       </c>
       <c r="C18">
-        <v>1789633384.68437</v>
+        <v>1789709326.71765</v>
       </c>
       <c r="D18">
-        <v>24456.622863756</v>
+        <v>23496.9785109574</v>
+      </c>
+      <c r="E18">
+        <v>3.002425906844</v>
       </c>
       <c r="F18">
-        <v>1789633384.68437</v>
+        <v>1789709326.71765</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_4</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_4</t>
         </is>
       </c>
       <c r="B19">
@@ -737,7 +737,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_17</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_17</t>
         </is>
       </c>
       <c r="B20">
@@ -756,7 +756,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GBM_1_AutoML_2_20240525_22650</t>
+          <t>GBM_1_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B21">
@@ -775,7 +775,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_22</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_22</t>
         </is>
       </c>
       <c r="B22">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_1_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_BestOfFamily_1_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B23">
@@ -813,7 +813,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_11</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_11</t>
         </is>
       </c>
       <c r="B24">
@@ -832,7 +832,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_7</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_7</t>
         </is>
       </c>
       <c r="B25">
@@ -851,7 +851,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>GBM_5_AutoML_2_20240525_22650</t>
+          <t>GBM_5_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B26">
@@ -870,7 +870,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_10</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_10</t>
         </is>
       </c>
       <c r="B27">
@@ -889,7 +889,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_24</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_24</t>
         </is>
       </c>
       <c r="B28">
@@ -908,7 +908,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_13</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_13</t>
         </is>
       </c>
       <c r="B29">
@@ -927,7 +927,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_6</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_6</t>
         </is>
       </c>
       <c r="B30">
@@ -946,7 +946,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_14</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_14</t>
         </is>
       </c>
       <c r="B31">
@@ -965,29 +965,29 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_5_AutoML_2_20240525_22650</t>
+          <t>StackedEnsemble_BestOfFamily_5_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B32">
-        <v>42803.9098656799</v>
+        <v>42808.5852150732</v>
       </c>
       <c r="C32">
-        <v>1832174699.78925</v>
+        <v>1832574968.11619</v>
       </c>
       <c r="D32">
-        <v>24184.6363352569</v>
+        <v>24166.6552363412</v>
       </c>
       <c r="E32">
-        <v>3.00370080057606</v>
+        <v>3.00193317106895</v>
       </c>
       <c r="F32">
-        <v>1832174699.78925</v>
+        <v>1832574968.11619</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_5</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_5</t>
         </is>
       </c>
       <c r="B33">
@@ -1006,7 +1006,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_8</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_8</t>
         </is>
       </c>
       <c r="B34">
@@ -1025,102 +1025,102 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_21</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_50</t>
         </is>
       </c>
       <c r="B35">
-        <v>42986.584473911</v>
+        <v>42943.208398986</v>
       </c>
       <c r="C35">
-        <v>1847846444.73269</v>
+        <v>1844119147.59874</v>
       </c>
       <c r="D35">
-        <v>25293.4468413183</v>
+        <v>24869.8716158882</v>
       </c>
       <c r="F35">
-        <v>1847846444.73269</v>
+        <v>1844119147.59874</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_15</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_21</t>
         </is>
       </c>
       <c r="B36">
-        <v>42996.2334460932</v>
+        <v>42986.584473911</v>
       </c>
       <c r="C36">
-        <v>1848676090.55095</v>
+        <v>1847846444.73269</v>
       </c>
       <c r="D36">
-        <v>25059.7531429502</v>
+        <v>25293.4468413183</v>
       </c>
       <c r="F36">
-        <v>1848676090.55095</v>
+        <v>1847846444.73269</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>GBM_4_AutoML_2_20240525_22650</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_15</t>
         </is>
       </c>
       <c r="B37">
-        <v>43000.4738309286</v>
+        <v>42996.2334460932</v>
       </c>
       <c r="C37">
-        <v>1849040749.68437</v>
+        <v>1848676090.55095</v>
       </c>
       <c r="D37">
-        <v>24578.2327437266</v>
+        <v>25059.7531429502</v>
       </c>
       <c r="F37">
-        <v>1849040749.68437</v>
+        <v>1848676090.55095</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_50</t>
+          <t>GBM_4_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B38">
-        <v>43473.0703166419</v>
+        <v>43000.4738309286</v>
       </c>
       <c r="C38">
-        <v>1889907842.75569</v>
+        <v>1849040749.68437</v>
       </c>
       <c r="D38">
-        <v>25246.7617476476</v>
+        <v>24578.2327437266</v>
       </c>
       <c r="F38">
-        <v>1889907842.75569</v>
+        <v>1849040749.68437</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_49</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_49</t>
         </is>
       </c>
       <c r="B39">
-        <v>43801.8663105715</v>
+        <v>43782.8859403507</v>
       </c>
       <c r="C39">
-        <v>1918603492.28918</v>
+        <v>1916941101.26576</v>
       </c>
       <c r="D39">
-        <v>25526.3440327844</v>
+        <v>25513.6696901049</v>
       </c>
       <c r="F39">
-        <v>1918603492.28918</v>
+        <v>1916941101.26576</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_18</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_18</t>
         </is>
       </c>
       <c r="B40">
@@ -1139,7 +1139,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_19</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_19</t>
         </is>
       </c>
       <c r="B41">
@@ -1158,7 +1158,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>DRF_1_AutoML_2_20240525_22650</t>
+          <t>DRF_1_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B42">
@@ -1180,7 +1180,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>XRT_1_AutoML_2_20240525_22650</t>
+          <t>XRT_1_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B43">
@@ -1202,7 +1202,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_23</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_23</t>
         </is>
       </c>
       <c r="B44">
@@ -1221,7 +1221,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_3</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_3</t>
         </is>
       </c>
       <c r="B45">
@@ -1240,7 +1240,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_12</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_12</t>
         </is>
       </c>
       <c r="B46">
@@ -1262,7 +1262,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_9</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_9</t>
         </is>
       </c>
       <c r="B47">
@@ -1281,253 +1281,253 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_1_AutoML_2_20240525_22650_model_1</t>
+          <t>DeepLearning_grid_1_AutoML_1_20240525_142933_model_1</t>
         </is>
       </c>
       <c r="B48">
-        <v>47804.244450427</v>
+        <v>48181.4447224675</v>
       </c>
       <c r="C48">
-        <v>2285245787.47618</v>
+        <v>2321451615.54419</v>
       </c>
       <c r="D48">
-        <v>29765.8030496652</v>
+        <v>29822.1355951402</v>
       </c>
       <c r="F48">
-        <v>2285245787.47618</v>
+        <v>2321451615.54419</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_1_AutoML_2_20240525_22650_model_3</t>
+          <t>DeepLearning_grid_1_AutoML_1_20240525_142933_model_3</t>
         </is>
       </c>
       <c r="B49">
-        <v>47922.0853342052</v>
+        <v>48310.5829853662</v>
       </c>
       <c r="C49">
-        <v>2296526262.77885</v>
+        <v>2333912428.38596</v>
       </c>
       <c r="D49">
-        <v>30600.1391275753</v>
+        <v>29596.305746314</v>
       </c>
       <c r="F49">
-        <v>2296526262.77885</v>
+        <v>2333912428.38596</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DeepLearning_1_AutoML_2_20240525_22650</t>
+          <t>DeepLearning_1_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B50">
-        <v>49424.1793480849</v>
+        <v>49248.6750431834</v>
       </c>
       <c r="C50">
-        <v>2442749504.23166</v>
+        <v>2425431993.50907</v>
       </c>
       <c r="D50">
-        <v>31516.5988375553</v>
+        <v>31150.5162145537</v>
       </c>
       <c r="F50">
-        <v>2442749504.23166</v>
+        <v>2425431993.50907</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_2_AutoML_2_20240525_22650_model_3</t>
+          <t>DeepLearning_grid_1_AutoML_1_20240525_142933_model_4</t>
         </is>
       </c>
       <c r="B51">
-        <v>49424.2488439223</v>
+        <v>49364.875213671</v>
       </c>
       <c r="C51">
-        <v>2442756373.78595</v>
+        <v>2436890904.86131</v>
       </c>
       <c r="D51">
-        <v>31729.8217355375</v>
-      </c>
-      <c r="E51">
-        <v>3.22828764357369</v>
+        <v>31326.4734378545</v>
       </c>
       <c r="F51">
-        <v>2442756373.78595</v>
+        <v>2436890904.86131</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_1_AutoML_2_20240525_22650_model_4</t>
+          <t>GBM_grid_1_AutoML_1_20240525_142933_model_51</t>
         </is>
       </c>
       <c r="B52">
-        <v>49811.5577599478</v>
+        <v>49547.0324099614</v>
       </c>
       <c r="C52">
-        <v>2481191286.47262</v>
+        <v>2454908420.63377</v>
       </c>
       <c r="D52">
-        <v>31686.8491191038</v>
+        <v>31956.4374772204</v>
+      </c>
+      <c r="E52">
+        <v>3.32808142069402</v>
       </c>
       <c r="F52">
-        <v>2481191286.47262</v>
+        <v>2454908420.63377</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_1_AutoML_2_20240525_22650_model_9</t>
+          <t>DeepLearning_grid_3_AutoML_1_20240525_142933_model_3</t>
         </is>
       </c>
       <c r="B53">
-        <v>50551.4984784073</v>
+        <v>49547.6627480308</v>
       </c>
       <c r="C53">
-        <v>2555453998.41241</v>
+        <v>2454970883.7926</v>
       </c>
       <c r="D53">
-        <v>32482.4221167918</v>
+        <v>32115.6869891946</v>
+      </c>
+      <c r="E53">
+        <v>3.26901564396188</v>
       </c>
       <c r="F53">
-        <v>2555453998.41241</v>
+        <v>2454970883.7926</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_3_AutoML_2_20240525_22650_model_2</t>
+          <t>DeepLearning_grid_2_AutoML_1_20240525_142933_model_3</t>
         </is>
       </c>
       <c r="B54">
-        <v>54073.4364316675</v>
+        <v>49600.1662468616</v>
       </c>
       <c r="C54">
-        <v>2923936527.52959</v>
+        <v>2460176491.71631</v>
       </c>
       <c r="D54">
-        <v>38921.6938049522</v>
+        <v>32200.2549882723</v>
       </c>
       <c r="E54">
-        <v>3.49135766609645</v>
+        <v>3.25126344450862</v>
       </c>
       <c r="F54">
-        <v>2923936527.52959</v>
+        <v>2460176491.71631</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_1_AutoML_2_20240525_22650_model_2</t>
+          <t>DeepLearning_grid_1_AutoML_1_20240525_142933_model_9</t>
         </is>
       </c>
       <c r="B55">
-        <v>54565.6595939865</v>
+        <v>51178.1784954011</v>
       </c>
       <c r="C55">
-        <v>2977411206.92681</v>
+        <v>2619205954.10713</v>
       </c>
       <c r="D55">
-        <v>34252.5187453923</v>
+        <v>32348.6244768845</v>
       </c>
       <c r="F55">
-        <v>2977411206.92681</v>
+        <v>2619205954.10713</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_2_AutoML_2_20240525_22650_model_2</t>
+          <t>DeepLearning_grid_1_AutoML_1_20240525_142933_model_2</t>
         </is>
       </c>
       <c r="B56">
-        <v>55238.4819415812</v>
+        <v>53643.635548867</v>
       </c>
       <c r="C56">
-        <v>3051289887.21039</v>
+        <v>2877639634.89967</v>
       </c>
       <c r="D56">
-        <v>41259.7534453813</v>
-      </c>
-      <c r="E56">
-        <v>3.53873108579779</v>
+        <v>33917.388149328</v>
       </c>
       <c r="F56">
-        <v>3051289887.21039</v>
+        <v>2877639634.89967</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_3_AutoML_2_20240525_22650_model_1</t>
+          <t>DeepLearning_grid_3_AutoML_1_20240525_142933_model_2</t>
         </is>
       </c>
       <c r="B57">
-        <v>58117.5679718396</v>
+        <v>54407.399043952</v>
       </c>
       <c r="C57">
-        <v>3377651706.96139</v>
+        <v>2960165070.72783</v>
       </c>
       <c r="D57">
-        <v>46780.4941438151</v>
+        <v>39296.08939981</v>
       </c>
       <c r="E57">
-        <v>3.61788155612997</v>
+        <v>3.50364695768501</v>
       </c>
       <c r="F57">
-        <v>3377651706.96139</v>
+        <v>2960165070.72783</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_2_20240525_22650_model_51</t>
+          <t>DeepLearning_grid_2_AutoML_1_20240525_142933_model_2</t>
         </is>
       </c>
       <c r="B58">
-        <v>59238.3475087251</v>
+        <v>55202.7299580206</v>
       </c>
       <c r="C58">
-        <v>3509181815.56447</v>
+        <v>3047341394.81815</v>
       </c>
       <c r="D58">
-        <v>41705.6832865386</v>
+        <v>40137.7739927866</v>
       </c>
       <c r="E58">
-        <v>3.50108810137939</v>
+        <v>3.5102735467676</v>
       </c>
       <c r="F58">
-        <v>3509181815.56447</v>
+        <v>3047341394.81815</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_2_AutoML_2_20240525_22650_model_1</t>
+          <t>DeepLearning_grid_3_AutoML_1_20240525_142933_model_1</t>
         </is>
       </c>
       <c r="B59">
-        <v>60194.3340586933</v>
+        <v>56368.672361003</v>
       </c>
       <c r="C59">
-        <v>3623357852.76957</v>
+        <v>3177427223.7421</v>
       </c>
       <c r="D59">
-        <v>48949.9374622048</v>
+        <v>44342.1504942428</v>
       </c>
       <c r="E59">
-        <v>3.64840079049955</v>
+        <v>3.58504348729328</v>
       </c>
       <c r="F59">
-        <v>3623357852.76957</v>
+        <v>3177427223.7421</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>GLM_1_AutoML_2_20240525_22650</t>
+          <t>GLM_1_AutoML_1_20240525_142933</t>
         </is>
       </c>
       <c r="B60">
@@ -1544,6 +1544,28 @@
       </c>
       <c r="F60">
         <v>3773659177.41499</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_2_AutoML_1_20240525_142933_model_1</t>
+        </is>
+      </c>
+      <c r="B61">
+        <v>61945.7377602217</v>
+      </c>
+      <c r="C61">
+        <v>3837274426.65815</v>
+      </c>
+      <c r="D61">
+        <v>51122.2305832154</v>
+      </c>
+      <c r="E61">
+        <v>3.6626927483468</v>
+      </c>
+      <c r="F61">
+        <v>3837274426.65815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor preprocessing steps in textmining_bfh_tweets_group_10.Rmd
</commit_message>
<xml_diff>
--- a/3.Applied-Supervised-Learning-Groupwork/trained_ML_models.xlsx
+++ b/3.Applied-Supervised-Learning-Groupwork/trained_ML_models.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -392,1180 +392,2016 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_4_AutoML_1_20240525_142933</t>
+          <t>StackedEnsemble_AllModels_5_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B2">
-        <v>41418.1011303562</v>
+        <v>25953.6764765662</v>
       </c>
       <c r="C2">
-        <v>1715459101.24441</v>
+        <v>673593322.650264</v>
       </c>
       <c r="D2">
-        <v>23277.7675710024</v>
+        <v>17854.9934565678</v>
+      </c>
+      <c r="E2">
+        <v>2.95767168405498</v>
       </c>
       <c r="F2">
-        <v>1715459101.24441</v>
+        <v>673593322.650264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_6_AutoML_1_20240525_142933</t>
+          <t>StackedEnsemble_AllModels_6_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B3">
-        <v>41418.909908912</v>
+        <v>25964.9013746912</v>
       </c>
       <c r="C3">
-        <v>1715526098.04257</v>
+        <v>674176103.397439</v>
       </c>
       <c r="D3">
-        <v>23255.0450001868</v>
+        <v>18009.4816267214</v>
       </c>
       <c r="F3">
-        <v>1715526098.04257</v>
+        <v>674176103.397439</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>StackedEnsemble_Best1000_1_AutoML_1_20240525_142933</t>
+          <t>StackedEnsemble_Best1000_1_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B4">
-        <v>41454.8147379177</v>
+        <v>25973.3417150623</v>
       </c>
       <c r="C4">
-        <v>1718501664.95508</v>
+        <v>674614479.847396</v>
       </c>
       <c r="D4">
-        <v>23294.3303148232</v>
+        <v>18009.8901258163</v>
       </c>
       <c r="F4">
-        <v>1718501664.95508</v>
+        <v>674614479.847396</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_3_AutoML_1_20240525_142933</t>
+          <t>StackedEnsemble_AllModels_3_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B5">
-        <v>41491.707182241</v>
+        <v>25975.7267172851</v>
       </c>
       <c r="C5">
-        <v>1721561764.89683</v>
+        <v>674738378.491079</v>
       </c>
       <c r="D5">
-        <v>23316.1016916845</v>
+        <v>18018.1599808612</v>
       </c>
       <c r="F5">
-        <v>1721561764.89683</v>
+        <v>674738378.491079</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_2_AutoML_1_20240525_142933</t>
+          <t>StackedEnsemble_AllModels_4_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B6">
-        <v>41618.6843645661</v>
+        <v>25977.457281805</v>
       </c>
       <c r="C6">
-        <v>1732114888.23738</v>
+        <v>674828286.828006</v>
       </c>
       <c r="D6">
-        <v>23401.3032092364</v>
+        <v>18011.6860480138</v>
       </c>
       <c r="F6">
-        <v>1732114888.23738</v>
+        <v>674828286.828006</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_1_AutoML_1_20240525_142933</t>
+          <t>StackedEnsemble_AllModels_2_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B7">
-        <v>41628.1194400005</v>
+        <v>26139.0539126436</v>
       </c>
       <c r="C7">
-        <v>1732900328.11095</v>
+        <v>683250139.448089</v>
       </c>
       <c r="D7">
-        <v>23434.4294376615</v>
+        <v>18107.7455046202</v>
       </c>
       <c r="F7">
-        <v>1732900328.11095</v>
+        <v>683250139.448089</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GBM_2_AutoML_1_20240525_142933</t>
+          <t>StackedEnsemble_AllModels_1_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B8">
-        <v>42029.6345134108</v>
+        <v>26195.5107694089</v>
       </c>
       <c r="C8">
-        <v>1766490177.33089</v>
+        <v>686204784.470216</v>
       </c>
       <c r="D8">
-        <v>23875.5597525215</v>
+        <v>18135.0393528394</v>
       </c>
       <c r="F8">
-        <v>1766490177.33089</v>
+        <v>686204784.470216</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_2_AutoML_1_20240525_142933</t>
+          <t>StackedEnsemble_BestOfFamily_4_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B9">
-        <v>42041.3717169267</v>
+        <v>26445.1230487547</v>
       </c>
       <c r="C9">
-        <v>1767476935.8408</v>
+        <v>699344533.063778</v>
       </c>
       <c r="D9">
-        <v>23817.9704746173</v>
+        <v>18373.1510775453</v>
       </c>
       <c r="F9">
-        <v>1767476935.8408</v>
+        <v>699344533.063778</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_4_AutoML_1_20240525_142933</t>
+          <t>StackedEnsemble_BestOfFamily_2_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B10">
-        <v>42046.6137318345</v>
+        <v>26446.6304012854</v>
       </c>
       <c r="C10">
-        <v>1767917726.31409</v>
+        <v>699424259.582193</v>
       </c>
       <c r="D10">
-        <v>23824.0538579689</v>
+        <v>18376.0625647871</v>
       </c>
       <c r="F10">
-        <v>1767917726.31409</v>
+        <v>699424259.582193</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_3_AutoML_1_20240525_142933</t>
+          <t>StackedEnsemble_BestOfFamily_3_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B11">
-        <v>42049.0451578926</v>
+        <v>26447.7592112792</v>
       </c>
       <c r="C11">
-        <v>1768122198.69049</v>
+        <v>699483967.297804</v>
       </c>
       <c r="D11">
-        <v>23822.1606639521</v>
+        <v>18375.2250871511</v>
       </c>
       <c r="F11">
-        <v>1768122198.69049</v>
+        <v>699483967.297804</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_6_AutoML_1_20240525_142933</t>
+          <t>GBM_2_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B12">
-        <v>42076.909972133</v>
+        <v>26448.6847880018</v>
       </c>
       <c r="C12">
-        <v>1770466352.80299</v>
+        <v>699532927.01508</v>
       </c>
       <c r="D12">
-        <v>23846.2304531303</v>
+        <v>18424.6251172095</v>
       </c>
       <c r="F12">
-        <v>1770466352.80299</v>
+        <v>699532927.01508</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_16</t>
+          <t>StackedEnsemble_BestOfFamily_6_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B13">
-        <v>42094.3089312768</v>
+        <v>26449.4568428325</v>
       </c>
       <c r="C13">
-        <v>1771930844.40177</v>
+        <v>699573767.280857</v>
       </c>
       <c r="D13">
-        <v>24132.0792575695</v>
+        <v>18385.7294774588</v>
       </c>
       <c r="F13">
-        <v>1771930844.40177</v>
+        <v>699573767.280857</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_2</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_50</t>
         </is>
       </c>
       <c r="B14">
-        <v>42133.026462265</v>
+        <v>26497.9481578339</v>
       </c>
       <c r="C14">
-        <v>1775191918.86992</v>
+        <v>702141256.575251</v>
       </c>
       <c r="D14">
-        <v>23931.6386121976</v>
+        <v>18430.5243888819</v>
       </c>
       <c r="F14">
-        <v>1775191918.86992</v>
+        <v>702141256.575251</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GBM_3_AutoML_1_20240525_142933</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_40</t>
         </is>
       </c>
       <c r="B15">
-        <v>42140.6706663195</v>
+        <v>26528.2635503011</v>
       </c>
       <c r="C15">
-        <v>1775836124.2072</v>
+        <v>703748766.994235</v>
       </c>
       <c r="D15">
-        <v>23978.7603562361</v>
+        <v>18568.5033949879</v>
       </c>
       <c r="F15">
-        <v>1775836124.2072</v>
+        <v>703748766.994235</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_1</t>
+          <t>GBM_3_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B16">
-        <v>42205.2072702395</v>
+        <v>26566.2077443975</v>
       </c>
       <c r="C16">
-        <v>1781279520.72388</v>
+        <v>705763393.918488</v>
       </c>
       <c r="D16">
-        <v>24176.5340737375</v>
+        <v>18516.349918185</v>
       </c>
       <c r="F16">
-        <v>1781279520.72388</v>
+        <v>705763393.918488</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_20</t>
+          <t>StackedEnsemble_BestOfFamily_5_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B17">
-        <v>42304.0587258997</v>
+        <v>26617.439901323</v>
       </c>
       <c r="C17">
-        <v>1789633384.68437</v>
+        <v>708488106.900543</v>
       </c>
       <c r="D17">
-        <v>24456.622863756</v>
+        <v>18429.5139435944</v>
+      </c>
+      <c r="E17">
+        <v>2.96661257569309</v>
       </c>
       <c r="F17">
-        <v>1789633384.68437</v>
+        <v>708488106.900543</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_5_AutoML_1_20240525_142933</t>
+          <t>GBM_5_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B18">
-        <v>42304.9562902227</v>
+        <v>26635.2381552266</v>
       </c>
       <c r="C18">
-        <v>1789709326.71765</v>
+        <v>709435911.585636</v>
       </c>
       <c r="D18">
-        <v>23496.9785109574</v>
-      </c>
-      <c r="E18">
-        <v>3.002425906844</v>
+        <v>18638.0825366145</v>
       </c>
       <c r="F18">
-        <v>1789709326.71765</v>
+        <v>709435911.585636</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_4</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_2</t>
         </is>
       </c>
       <c r="B19">
-        <v>42348.1428127604</v>
+        <v>26635.9521925523</v>
       </c>
       <c r="C19">
-        <v>1793365199.68995</v>
+        <v>709473949.203933</v>
       </c>
       <c r="D19">
-        <v>24365.1660316765</v>
+        <v>18566.2289817685</v>
       </c>
       <c r="F19">
-        <v>1793365199.68995</v>
+        <v>709473949.203933</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_17</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_11</t>
         </is>
       </c>
       <c r="B20">
-        <v>42366.5997539428</v>
+        <v>26646.819587869</v>
       </c>
       <c r="C20">
-        <v>1794928774.71079</v>
+        <v>710052994.14844</v>
       </c>
       <c r="D20">
-        <v>24259.6904492552</v>
+        <v>18595.7805973152</v>
       </c>
       <c r="F20">
-        <v>1794928774.71079</v>
+        <v>710052994.14844</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GBM_1_AutoML_1_20240525_142933</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_16</t>
         </is>
       </c>
       <c r="B21">
-        <v>42372.9949628573</v>
+        <v>26681.8595604156</v>
       </c>
       <c r="C21">
-        <v>1795470702.12233</v>
+        <v>711921629.6017441</v>
       </c>
       <c r="D21">
-        <v>24115.0317274371</v>
+        <v>18879.9128485333</v>
       </c>
       <c r="F21">
-        <v>1795470702.12233</v>
+        <v>711921629.6017441</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_22</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_54</t>
         </is>
       </c>
       <c r="B22">
-        <v>42391.579501679</v>
+        <v>26718.9351713573</v>
       </c>
       <c r="C22">
-        <v>1797046012.64717</v>
+        <v>713901496.6911941</v>
       </c>
       <c r="D22">
-        <v>24507.1048461905</v>
+        <v>18758.0875770022</v>
       </c>
       <c r="F22">
-        <v>1797046012.64717</v>
+        <v>713901496.6911941</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_1_AutoML_1_20240525_142933</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_66</t>
         </is>
       </c>
       <c r="B23">
-        <v>42402.3460979994</v>
+        <v>26733.1255085381</v>
       </c>
       <c r="C23">
-        <v>1797958954.61453</v>
+        <v>714659999.455253</v>
       </c>
       <c r="D23">
-        <v>24140.9436708668</v>
+        <v>18807.1078602155</v>
       </c>
       <c r="F23">
-        <v>1797958954.61453</v>
+        <v>714659999.455253</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_11</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_1</t>
         </is>
       </c>
       <c r="B24">
-        <v>42410.8716962523</v>
+        <v>26751.8348594465</v>
       </c>
       <c r="C24">
-        <v>1798682038.03597</v>
+        <v>715660668.347095</v>
       </c>
       <c r="D24">
-        <v>24213.7547529863</v>
+        <v>18893.1045520578</v>
       </c>
       <c r="F24">
-        <v>1798682038.03597</v>
+        <v>715660668.347095</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_7</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_13</t>
         </is>
       </c>
       <c r="B25">
-        <v>42439.4250212029</v>
+        <v>26759.0645238962</v>
       </c>
       <c r="C25">
-        <v>1801104796.1303</v>
+        <v>716047534.1940399</v>
       </c>
       <c r="D25">
-        <v>24290.0408611731</v>
+        <v>18759.5919927039</v>
       </c>
       <c r="F25">
-        <v>1801104796.1303</v>
+        <v>716047534.1940399</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>GBM_5_AutoML_1_20240525_142933</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_71</t>
         </is>
       </c>
       <c r="B26">
-        <v>42448.3619570532</v>
+        <v>26761.1266089222</v>
       </c>
       <c r="C26">
-        <v>1801863432.83701</v>
+        <v>716157897.3787659</v>
       </c>
       <c r="D26">
-        <v>24162.7562446711</v>
+        <v>18678.2676288795</v>
       </c>
       <c r="F26">
-        <v>1801863432.83701</v>
+        <v>716157897.3787659</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_10</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_67</t>
         </is>
       </c>
       <c r="B27">
-        <v>42475.40090003</v>
+        <v>26784.9948340399</v>
       </c>
       <c r="C27">
-        <v>1804159681.61827</v>
+        <v>717435948.259546</v>
       </c>
       <c r="D27">
-        <v>24323.0045118147</v>
+        <v>18701.5843091421</v>
       </c>
       <c r="F27">
-        <v>1804159681.61827</v>
+        <v>717435948.259546</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_24</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_17</t>
         </is>
       </c>
       <c r="B28">
-        <v>42476.2854069832</v>
+        <v>26792.1338909229</v>
       </c>
       <c r="C28">
-        <v>1804234821.97549</v>
+        <v>717818438.429137</v>
       </c>
       <c r="D28">
-        <v>24291.7435823815</v>
+        <v>18816.0197141674</v>
       </c>
       <c r="F28">
-        <v>1804234821.97549</v>
+        <v>717818438.429137</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_13</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_14</t>
         </is>
       </c>
       <c r="B29">
-        <v>42615.8836539974</v>
+        <v>26902.4248598273</v>
       </c>
       <c r="C29">
-        <v>1816113539.61104</v>
+        <v>723740463.3386559</v>
       </c>
       <c r="D29">
-        <v>24391.5350638734</v>
+        <v>19017.389143322</v>
       </c>
       <c r="F29">
-        <v>1816113539.61104</v>
+        <v>723740463.3386559</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_6</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_4</t>
         </is>
       </c>
       <c r="B30">
-        <v>42763.4805331233</v>
+        <v>26919.7291259043</v>
       </c>
       <c r="C30">
-        <v>1828715267.30681</v>
+        <v>724671816.212063</v>
       </c>
       <c r="D30">
-        <v>24525.7079795011</v>
+        <v>18955.0313269183</v>
       </c>
       <c r="F30">
-        <v>1828715267.30681</v>
+        <v>724671816.212063</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_14</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_24</t>
         </is>
       </c>
       <c r="B31">
-        <v>42776.9577986585</v>
+        <v>26932.7932984761</v>
       </c>
       <c r="C31">
-        <v>1829868118.50821</v>
+        <v>725375354.858438</v>
       </c>
       <c r="D31">
-        <v>24831.4854243442</v>
+        <v>18828.1444311479</v>
       </c>
       <c r="F31">
-        <v>1829868118.50821</v>
+        <v>725375354.858438</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_5_AutoML_1_20240525_142933</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_5</t>
         </is>
       </c>
       <c r="B32">
-        <v>42808.5852150732</v>
+        <v>26949.6451511743</v>
       </c>
       <c r="C32">
-        <v>1832574968.11619</v>
+        <v>726283373.774215</v>
       </c>
       <c r="D32">
-        <v>24166.6552363412</v>
-      </c>
-      <c r="E32">
-        <v>3.00193317106895</v>
+        <v>18879.6434438751</v>
       </c>
       <c r="F32">
-        <v>1832574968.11619</v>
+        <v>726283373.774215</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_5</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_7</t>
         </is>
       </c>
       <c r="B33">
-        <v>42812.4346303333</v>
+        <v>26968.3315413661</v>
       </c>
       <c r="C33">
-        <v>1832904558.97656</v>
+        <v>727290906.125043</v>
       </c>
       <c r="D33">
-        <v>24528.8477730665</v>
+        <v>18958.861590561</v>
       </c>
       <c r="F33">
-        <v>1832904558.97656</v>
+        <v>727290906.125043</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_8</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_47</t>
         </is>
       </c>
       <c r="B34">
-        <v>42909.7099556486</v>
+        <v>26988.9752349013</v>
       </c>
       <c r="C34">
-        <v>1841243208.47789</v>
+        <v>728404784.230116</v>
       </c>
       <c r="D34">
-        <v>24669.0530292245</v>
+        <v>19043.5406554007</v>
       </c>
       <c r="F34">
-        <v>1841243208.47789</v>
+        <v>728404784.230116</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_50</t>
+          <t>GBM_4_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B35">
-        <v>42943.208398986</v>
+        <v>27009.5972794545</v>
       </c>
       <c r="C35">
-        <v>1844119147.59874</v>
+        <v>729518345.198313</v>
       </c>
       <c r="D35">
-        <v>24869.8716158882</v>
+        <v>18917.8452566798</v>
       </c>
       <c r="F35">
-        <v>1844119147.59874</v>
+        <v>729518345.198313</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_21</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_20</t>
         </is>
       </c>
       <c r="B36">
-        <v>42986.584473911</v>
+        <v>27014.6316056646</v>
       </c>
       <c r="C36">
-        <v>1847846444.73269</v>
+        <v>729790320.789775</v>
       </c>
       <c r="D36">
-        <v>25293.4468413183</v>
+        <v>19184.5637520741</v>
       </c>
       <c r="F36">
-        <v>1847846444.73269</v>
+        <v>729790320.789775</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_15</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_8</t>
         </is>
       </c>
       <c r="B37">
-        <v>42996.2334460932</v>
+        <v>27030.650949518</v>
       </c>
       <c r="C37">
-        <v>1848676090.55095</v>
+        <v>730656090.754676</v>
       </c>
       <c r="D37">
-        <v>25059.7531429502</v>
+        <v>18840.8898473663</v>
       </c>
       <c r="F37">
-        <v>1848676090.55095</v>
+        <v>730656090.754676</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>GBM_4_AutoML_1_20240525_142933</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_6</t>
         </is>
       </c>
       <c r="B38">
-        <v>43000.4738309286</v>
+        <v>27034.5406810572</v>
       </c>
       <c r="C38">
-        <v>1849040749.68437</v>
+        <v>730866389.835735</v>
       </c>
       <c r="D38">
-        <v>24578.2327437266</v>
+        <v>18972.9566349748</v>
       </c>
       <c r="F38">
-        <v>1849040749.68437</v>
+        <v>730866389.835735</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_49</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_27</t>
         </is>
       </c>
       <c r="B39">
-        <v>43782.8859403507</v>
+        <v>27053.8772873156</v>
       </c>
       <c r="C39">
-        <v>1916941101.26576</v>
+        <v>731912276.2771291</v>
       </c>
       <c r="D39">
-        <v>25513.6696901049</v>
+        <v>19124.6560640986</v>
       </c>
       <c r="F39">
-        <v>1916941101.26576</v>
+        <v>731912276.2771291</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_18</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_70</t>
         </is>
       </c>
       <c r="B40">
-        <v>43804.8410314878</v>
+        <v>27071.0460146</v>
       </c>
       <c r="C40">
-        <v>1918864097.79391</v>
+        <v>732841532.324592</v>
       </c>
       <c r="D40">
-        <v>25995.1836862335</v>
+        <v>18934.2866406056</v>
       </c>
       <c r="F40">
-        <v>1918864097.79391</v>
+        <v>732841532.324592</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_19</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_32</t>
         </is>
       </c>
       <c r="B41">
-        <v>43831.6492010863</v>
+        <v>27124.7776196183</v>
       </c>
       <c r="C41">
-        <v>1921213471.68709</v>
+        <v>735753560.913748</v>
       </c>
       <c r="D41">
-        <v>25515.8408216475</v>
+        <v>18982.0206388183</v>
       </c>
       <c r="F41">
-        <v>1921213471.68709</v>
+        <v>735753560.913748</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>DRF_1_AutoML_1_20240525_142933</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_22</t>
         </is>
       </c>
       <c r="B42">
-        <v>44145.5036721869</v>
+        <v>27158.9178829692</v>
       </c>
       <c r="C42">
-        <v>1948825494.47107</v>
+        <v>737606820.573864</v>
       </c>
       <c r="D42">
-        <v>26193.814973678</v>
-      </c>
-      <c r="E42">
-        <v>3.05507950360403</v>
+        <v>19320.2249906561</v>
       </c>
       <c r="F42">
-        <v>1948825494.47107</v>
+        <v>737606820.573864</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>XRT_1_AutoML_1_20240525_142933</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_44</t>
         </is>
       </c>
       <c r="B43">
-        <v>44609.879699531</v>
+        <v>27169.7109973133</v>
       </c>
       <c r="C43">
-        <v>1990041366.80663</v>
+        <v>738193195.677527</v>
       </c>
       <c r="D43">
-        <v>26775.42164167</v>
-      </c>
-      <c r="E43">
-        <v>3.08051854050194</v>
+        <v>19061.1283260652</v>
       </c>
       <c r="F43">
-        <v>1990041366.80663</v>
+        <v>738193195.677527</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_23</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_15</t>
         </is>
       </c>
       <c r="B44">
-        <v>44863.8158140551</v>
+        <v>27174.2149397502</v>
       </c>
       <c r="C44">
-        <v>2012761969.39746</v>
+        <v>738437957.591743</v>
       </c>
       <c r="D44">
-        <v>26801.7145896622</v>
+        <v>19362.2641369533</v>
       </c>
       <c r="F44">
-        <v>2012761969.39746</v>
+        <v>738437957.591743</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_3</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_46</t>
         </is>
       </c>
       <c r="B45">
-        <v>44883.2846153311</v>
+        <v>27174.8135234335</v>
       </c>
       <c r="C45">
-        <v>2014509237.86082</v>
+        <v>738470490.033385</v>
       </c>
       <c r="D45">
-        <v>26019.7797577181</v>
+        <v>19052.1837858502</v>
       </c>
       <c r="F45">
-        <v>2014509237.86082</v>
+        <v>738470490.033385</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_12</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_48</t>
         </is>
       </c>
       <c r="B46">
-        <v>45197.2559185494</v>
+        <v>27214.0911365117</v>
       </c>
       <c r="C46">
-        <v>2042791942.56685</v>
+        <v>740606756.386363</v>
       </c>
       <c r="D46">
-        <v>27315.0055620256</v>
-      </c>
-      <c r="E46">
-        <v>3.06843817267202</v>
+        <v>19216.9485521179</v>
       </c>
       <c r="F46">
-        <v>2042791942.56685</v>
+        <v>740606756.386363</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_9</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_59</t>
         </is>
       </c>
       <c r="B47">
-        <v>45760.7343493028</v>
+        <v>27292.7198854241</v>
       </c>
       <c r="C47">
-        <v>2094044808.18746</v>
+        <v>744892558.744223</v>
       </c>
       <c r="D47">
-        <v>27087.443849101</v>
+        <v>19088.576578518</v>
       </c>
       <c r="F47">
-        <v>2094044808.18746</v>
+        <v>744892558.744223</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_1_AutoML_1_20240525_142933_model_1</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_35</t>
         </is>
       </c>
       <c r="B48">
-        <v>48181.4447224675</v>
+        <v>27293.082224832</v>
       </c>
       <c r="C48">
-        <v>2321451615.54419</v>
+        <v>744912337.331439</v>
       </c>
       <c r="D48">
-        <v>29822.1355951402</v>
+        <v>19347.5793313203</v>
       </c>
       <c r="F48">
-        <v>2321451615.54419</v>
+        <v>744912337.331439</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_1_AutoML_1_20240525_142933_model_3</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_58</t>
         </is>
       </c>
       <c r="B49">
-        <v>48310.5829853662</v>
+        <v>27370.6080902144</v>
       </c>
       <c r="C49">
-        <v>2333912428.38596</v>
+        <v>749150187.228109</v>
       </c>
       <c r="D49">
-        <v>29596.305746314</v>
+        <v>19318.8395531854</v>
       </c>
       <c r="F49">
-        <v>2333912428.38596</v>
+        <v>749150187.228109</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DeepLearning_1_AutoML_1_20240525_142933</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_41</t>
         </is>
       </c>
       <c r="B50">
-        <v>49248.6750431834</v>
+        <v>27427.2518774566</v>
       </c>
       <c r="C50">
-        <v>2425431993.50907</v>
+        <v>752254145.549444</v>
       </c>
       <c r="D50">
-        <v>31150.5162145537</v>
+        <v>19486.7205030844</v>
       </c>
       <c r="F50">
-        <v>2425431993.50907</v>
+        <v>752254145.549444</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_1_AutoML_1_20240525_142933_model_4</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_30</t>
         </is>
       </c>
       <c r="B51">
-        <v>49364.875213671</v>
+        <v>27439.7105372804</v>
       </c>
       <c r="C51">
-        <v>2436890904.86131</v>
+        <v>752937714.3697391</v>
       </c>
       <c r="D51">
-        <v>31326.4734378545</v>
+        <v>19134.9828389745</v>
       </c>
       <c r="F51">
-        <v>2436890904.86131</v>
+        <v>752937714.3697391</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_1_20240525_142933_model_51</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_60</t>
         </is>
       </c>
       <c r="B52">
-        <v>49547.0324099614</v>
+        <v>27445.9876498188</v>
       </c>
       <c r="C52">
-        <v>2454908420.63377</v>
+        <v>753282238.074006</v>
       </c>
       <c r="D52">
-        <v>31956.4374772204</v>
-      </c>
-      <c r="E52">
-        <v>3.32808142069402</v>
+        <v>19335.4018074429</v>
       </c>
       <c r="F52">
-        <v>2454908420.63377</v>
+        <v>753282238.074006</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_3_AutoML_1_20240525_142933_model_3</t>
+          <t>StackedEnsemble_BestOfFamily_1_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B53">
-        <v>49547.6627480308</v>
+        <v>27457.0057155853</v>
       </c>
       <c r="C53">
-        <v>2454970883.7926</v>
+        <v>753887162.8656861</v>
       </c>
       <c r="D53">
-        <v>32115.6869891946</v>
-      </c>
-      <c r="E53">
-        <v>3.26901564396188</v>
+        <v>19153.6787885979</v>
       </c>
       <c r="F53">
-        <v>2454970883.7926</v>
+        <v>753887162.8656861</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_2_AutoML_1_20240525_142933_model_3</t>
+          <t>GBM_1_AutoML_3_20240527_104809</t>
         </is>
       </c>
       <c r="B54">
-        <v>49600.1662468616</v>
+        <v>27462.2819525765</v>
       </c>
       <c r="C54">
-        <v>2460176491.71631</v>
+        <v>754176930.04281</v>
       </c>
       <c r="D54">
-        <v>32200.2549882723</v>
-      </c>
-      <c r="E54">
-        <v>3.25126344450862</v>
+        <v>19183.2736384172</v>
       </c>
       <c r="F54">
-        <v>2460176491.71631</v>
+        <v>754176930.04281</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_1_AutoML_1_20240525_142933_model_9</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_45</t>
         </is>
       </c>
       <c r="B55">
-        <v>51178.1784954011</v>
+        <v>27562.4461922221</v>
       </c>
       <c r="C55">
-        <v>2619205954.10713</v>
+        <v>759688440.099141</v>
       </c>
       <c r="D55">
-        <v>32348.6244768845</v>
+        <v>19321.6619767985</v>
       </c>
       <c r="F55">
-        <v>2619205954.10713</v>
+        <v>759688440.099141</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_1_AutoML_1_20240525_142933_model_2</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_49</t>
         </is>
       </c>
       <c r="B56">
-        <v>53643.635548867</v>
+        <v>27637.5748985135</v>
       </c>
       <c r="C56">
-        <v>2877639634.89967</v>
+        <v>763835546.270945</v>
       </c>
       <c r="D56">
-        <v>33917.388149328</v>
+        <v>19681.1039691576</v>
       </c>
       <c r="F56">
-        <v>2877639634.89967</v>
+        <v>763835546.270945</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_3_AutoML_1_20240525_142933_model_2</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_10</t>
         </is>
       </c>
       <c r="B57">
-        <v>54407.399043952</v>
+        <v>27689.9821676463</v>
       </c>
       <c r="C57">
-        <v>2960165070.72783</v>
+        <v>766735112.444572</v>
       </c>
       <c r="D57">
-        <v>39296.08939981</v>
-      </c>
-      <c r="E57">
-        <v>3.50364695768501</v>
+        <v>19439.0977918421</v>
       </c>
       <c r="F57">
-        <v>2960165070.72783</v>
+        <v>766735112.444572</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_2_AutoML_1_20240525_142933_model_2</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_34</t>
         </is>
       </c>
       <c r="B58">
-        <v>55202.7299580206</v>
+        <v>27691.5180768571</v>
       </c>
       <c r="C58">
-        <v>3047341394.81815</v>
+        <v>766820173.400905</v>
       </c>
       <c r="D58">
-        <v>40137.7739927866</v>
-      </c>
-      <c r="E58">
-        <v>3.5102735467676</v>
+        <v>19345.9171915572</v>
       </c>
       <c r="F58">
-        <v>3047341394.81815</v>
+        <v>766820173.400905</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_3_AutoML_1_20240525_142933_model_1</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_19</t>
         </is>
       </c>
       <c r="B59">
-        <v>56368.672361003</v>
+        <v>27741.6994411372</v>
       </c>
       <c r="C59">
-        <v>3177427223.7421</v>
+        <v>769601887.882395</v>
       </c>
       <c r="D59">
-        <v>44342.1504942428</v>
-      </c>
-      <c r="E59">
-        <v>3.58504348729328</v>
+        <v>19611.8932864877</v>
       </c>
       <c r="F59">
-        <v>3177427223.7421</v>
+        <v>769601887.882395</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>GLM_1_AutoML_1_20240525_142933</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_25</t>
         </is>
       </c>
       <c r="B60">
-        <v>61430.1162087049</v>
+        <v>27747.8546991663</v>
       </c>
       <c r="C60">
-        <v>3773659177.41499</v>
+        <v>769943440.4060481</v>
       </c>
       <c r="D60">
-        <v>43792.2726414094</v>
-      </c>
-      <c r="E60">
-        <v>3.52876514711703</v>
+        <v>19722.0070910669</v>
       </c>
       <c r="F60">
-        <v>3773659177.41499</v>
+        <v>769943440.4060481</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>DeepLearning_grid_2_AutoML_1_20240525_142933_model_1</t>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_65</t>
         </is>
       </c>
       <c r="B61">
-        <v>61945.7377602217</v>
+        <v>27760.542322574</v>
       </c>
       <c r="C61">
-        <v>3837274426.65815</v>
+        <v>770647710.0434231</v>
       </c>
       <c r="D61">
-        <v>51122.2305832154</v>
-      </c>
-      <c r="E61">
-        <v>3.6626927483468</v>
+        <v>19813.2575891327</v>
       </c>
       <c r="F61">
-        <v>3837274426.65815</v>
+        <v>770647710.0434231</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_26</t>
+        </is>
+      </c>
+      <c r="B62">
+        <v>27784.490668406</v>
+      </c>
+      <c r="C62">
+        <v>771977921.702742</v>
+      </c>
+      <c r="D62">
+        <v>19681.6939316651</v>
+      </c>
+      <c r="F62">
+        <v>771977921.702742</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_55</t>
+        </is>
+      </c>
+      <c r="B63">
+        <v>27796.1043776928</v>
+      </c>
+      <c r="C63">
+        <v>772623418.575596</v>
+      </c>
+      <c r="D63">
+        <v>19580.6031428312</v>
+      </c>
+      <c r="F63">
+        <v>772623418.575596</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_39</t>
+        </is>
+      </c>
+      <c r="B64">
+        <v>27817.7507239784</v>
+      </c>
+      <c r="C64">
+        <v>773827255.341399</v>
+      </c>
+      <c r="D64">
+        <v>19692.3765594083</v>
+      </c>
+      <c r="F64">
+        <v>773827255.341399</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_53</t>
+        </is>
+      </c>
+      <c r="B65">
+        <v>27849.587481715</v>
+      </c>
+      <c r="C65">
+        <v>775599522.9016941</v>
+      </c>
+      <c r="D65">
+        <v>19549.6206862723</v>
+      </c>
+      <c r="F65">
+        <v>775599522.9016941</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_62</t>
+        </is>
+      </c>
+      <c r="B66">
+        <v>27884.6492399808</v>
+      </c>
+      <c r="C66">
+        <v>777553663.2367589</v>
+      </c>
+      <c r="D66">
+        <v>19725.1279113983</v>
+      </c>
+      <c r="F66">
+        <v>777553663.2367589</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_21</t>
+        </is>
+      </c>
+      <c r="B67">
+        <v>27890.8163397751</v>
+      </c>
+      <c r="C67">
+        <v>777897636.099064</v>
+      </c>
+      <c r="D67">
+        <v>19993.7378265136</v>
+      </c>
+      <c r="F67">
+        <v>777897636.099064</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_3</t>
+        </is>
+      </c>
+      <c r="B68">
+        <v>27965.4314370224</v>
+      </c>
+      <c r="C68">
+        <v>782065355.4588</v>
+      </c>
+      <c r="D68">
+        <v>19762.7450208328</v>
+      </c>
+      <c r="F68">
+        <v>782065355.4588</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_57</t>
+        </is>
+      </c>
+      <c r="B69">
+        <v>27991.8476353481</v>
+      </c>
+      <c r="C69">
+        <v>783543534.0405411</v>
+      </c>
+      <c r="D69">
+        <v>19840.182130707</v>
+      </c>
+      <c r="F69">
+        <v>783543534.0405411</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_56</t>
+        </is>
+      </c>
+      <c r="B70">
+        <v>27993.5021887644</v>
+      </c>
+      <c r="C70">
+        <v>783636164.792357</v>
+      </c>
+      <c r="D70">
+        <v>19697.5143610761</v>
+      </c>
+      <c r="F70">
+        <v>783636164.792357</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_51</t>
+        </is>
+      </c>
+      <c r="B71">
+        <v>27998.4568371644</v>
+      </c>
+      <c r="C71">
+        <v>783913585.262561</v>
+      </c>
+      <c r="D71">
+        <v>19745.1488225765</v>
+      </c>
+      <c r="F71">
+        <v>783913585.262561</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_52</t>
+        </is>
+      </c>
+      <c r="B72">
+        <v>28006.4164081842</v>
+      </c>
+      <c r="C72">
+        <v>784359360.028607</v>
+      </c>
+      <c r="D72">
+        <v>19823.2587798588</v>
+      </c>
+      <c r="F72">
+        <v>784359360.028607</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_33</t>
+        </is>
+      </c>
+      <c r="B73">
+        <v>28011.8174424215</v>
+      </c>
+      <c r="C73">
+        <v>784661916.427551</v>
+      </c>
+      <c r="D73">
+        <v>20111.6065573157</v>
+      </c>
+      <c r="F73">
+        <v>784661916.427551</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_37</t>
+        </is>
+      </c>
+      <c r="B74">
+        <v>28023.6027793018</v>
+      </c>
+      <c r="C74">
+        <v>785322312.732094</v>
+      </c>
+      <c r="D74">
+        <v>19730.6686503769</v>
+      </c>
+      <c r="F74">
+        <v>785322312.732094</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_36</t>
+        </is>
+      </c>
+      <c r="B75">
+        <v>28046.1899987905</v>
+      </c>
+      <c r="C75">
+        <v>786588773.448256</v>
+      </c>
+      <c r="D75">
+        <v>19991.2930852843</v>
+      </c>
+      <c r="F75">
+        <v>786588773.448256</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_43</t>
+        </is>
+      </c>
+      <c r="B76">
+        <v>28087.2745351917</v>
+      </c>
+      <c r="C76">
+        <v>788894990.815227</v>
+      </c>
+      <c r="D76">
+        <v>19894.308260214</v>
+      </c>
+      <c r="F76">
+        <v>788894990.815227</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_38</t>
+        </is>
+      </c>
+      <c r="B77">
+        <v>28092.8297127636</v>
+      </c>
+      <c r="C77">
+        <v>789207081.270336</v>
+      </c>
+      <c r="D77">
+        <v>19835.0800003641</v>
+      </c>
+      <c r="F77">
+        <v>789207081.270336</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_61</t>
+        </is>
+      </c>
+      <c r="B78">
+        <v>28165.4299087612</v>
+      </c>
+      <c r="C78">
+        <v>793291441.94534</v>
+      </c>
+      <c r="D78">
+        <v>19892.0732550875</v>
+      </c>
+      <c r="F78">
+        <v>793291441.94534</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_42</t>
+        </is>
+      </c>
+      <c r="B79">
+        <v>28199.9986289864</v>
+      </c>
+      <c r="C79">
+        <v>795239922.674835</v>
+      </c>
+      <c r="D79">
+        <v>20278.1753332654</v>
+      </c>
+      <c r="F79">
+        <v>795239922.674835</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_63</t>
+        </is>
+      </c>
+      <c r="B80">
+        <v>28228.0915732443</v>
+      </c>
+      <c r="C80">
+        <v>796825153.867466</v>
+      </c>
+      <c r="D80">
+        <v>19929.8103838264</v>
+      </c>
+      <c r="F80">
+        <v>796825153.867466</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_68</t>
+        </is>
+      </c>
+      <c r="B81">
+        <v>28258.1641667075</v>
+      </c>
+      <c r="C81">
+        <v>798523842.072593</v>
+      </c>
+      <c r="D81">
+        <v>20221.3325488025</v>
+      </c>
+      <c r="F81">
+        <v>798523842.072593</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_64</t>
+        </is>
+      </c>
+      <c r="B82">
+        <v>28271.9971908048</v>
+      </c>
+      <c r="C82">
+        <v>799305825.156872</v>
+      </c>
+      <c r="D82">
+        <v>20055.3046436175</v>
+      </c>
+      <c r="F82">
+        <v>799305825.156872</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_69</t>
+        </is>
+      </c>
+      <c r="B83">
+        <v>28275.5970841074</v>
+      </c>
+      <c r="C83">
+        <v>799509390.462783</v>
+      </c>
+      <c r="D83">
+        <v>20102.8909330691</v>
+      </c>
+      <c r="F83">
+        <v>799509390.462783</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_143</t>
+        </is>
+      </c>
+      <c r="B84">
+        <v>28406.7976960657</v>
+      </c>
+      <c r="C84">
+        <v>806946155.345206</v>
+      </c>
+      <c r="D84">
+        <v>20438.7873785014</v>
+      </c>
+      <c r="F84">
+        <v>806946155.345206</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_28</t>
+        </is>
+      </c>
+      <c r="B85">
+        <v>28445.6945333818</v>
+      </c>
+      <c r="C85">
+        <v>809157537.486467</v>
+      </c>
+      <c r="D85">
+        <v>20625.0437320281</v>
+      </c>
+      <c r="F85">
+        <v>809157537.486467</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_23</t>
+        </is>
+      </c>
+      <c r="B86">
+        <v>28512.4470335386</v>
+      </c>
+      <c r="C86">
+        <v>812959635.840345</v>
+      </c>
+      <c r="D86">
+        <v>20497.9063902774</v>
+      </c>
+      <c r="F86">
+        <v>812959635.840345</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_31</t>
+        </is>
+      </c>
+      <c r="B87">
+        <v>28700.1194058359</v>
+      </c>
+      <c r="C87">
+        <v>823696853.909241</v>
+      </c>
+      <c r="D87">
+        <v>20481.3610981412</v>
+      </c>
+      <c r="F87">
+        <v>823696853.909241</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_9</t>
+        </is>
+      </c>
+      <c r="B88">
+        <v>28994.6855035035</v>
+      </c>
+      <c r="C88">
+        <v>840691787.447075</v>
+      </c>
+      <c r="D88">
+        <v>20651.1665011592</v>
+      </c>
+      <c r="E88">
+        <v>2.99827664054663</v>
+      </c>
+      <c r="F88">
+        <v>840691787.447075</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_29</t>
+        </is>
+      </c>
+      <c r="B89">
+        <v>29053.9221738493</v>
+      </c>
+      <c r="C89">
+        <v>844130393.684094</v>
+      </c>
+      <c r="D89">
+        <v>20767.0606671311</v>
+      </c>
+      <c r="F89">
+        <v>844130393.684094</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>DRF_1_AutoML_3_20240527_104809</t>
+        </is>
+      </c>
+      <c r="B90">
+        <v>29056.0297884051</v>
+      </c>
+      <c r="C90">
+        <v>844252867.064684</v>
+      </c>
+      <c r="D90">
+        <v>20922.9173172925</v>
+      </c>
+      <c r="E90">
+        <v>3.02971297689165</v>
+      </c>
+      <c r="F90">
+        <v>844252867.064684</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_18</t>
+        </is>
+      </c>
+      <c r="B91">
+        <v>29106.1924671242</v>
+      </c>
+      <c r="C91">
+        <v>847170439.933277</v>
+      </c>
+      <c r="D91">
+        <v>21239.1948189763</v>
+      </c>
+      <c r="F91">
+        <v>847170439.933277</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>XRT_1_AutoML_3_20240527_104809</t>
+        </is>
+      </c>
+      <c r="B92">
+        <v>29280.5830655129</v>
+      </c>
+      <c r="C92">
+        <v>857352544.656399</v>
+      </c>
+      <c r="D92">
+        <v>21311.8507868639</v>
+      </c>
+      <c r="E92">
+        <v>3.05415933953721</v>
+      </c>
+      <c r="F92">
+        <v>857352544.656399</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_12</t>
+        </is>
+      </c>
+      <c r="B93">
+        <v>29385.9002333859</v>
+      </c>
+      <c r="C93">
+        <v>863531132.52651</v>
+      </c>
+      <c r="D93">
+        <v>21413.4247674038</v>
+      </c>
+      <c r="E93">
+        <v>3.04216380190729</v>
+      </c>
+      <c r="F93">
+        <v>863531132.52651</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_1_AutoML_3_20240527_104809_model_3</t>
+        </is>
+      </c>
+      <c r="B94">
+        <v>33793.6300336519</v>
+      </c>
+      <c r="C94">
+        <v>1142009430.85134</v>
+      </c>
+      <c r="D94">
+        <v>25532.6152585599</v>
+      </c>
+      <c r="F94">
+        <v>1142009430.85134</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_1_AutoML_3_20240527_104809_model_1</t>
+        </is>
+      </c>
+      <c r="B95">
+        <v>33844.4023968694</v>
+      </c>
+      <c r="C95">
+        <v>1145443573.60122</v>
+      </c>
+      <c r="D95">
+        <v>25295.1085297902</v>
+      </c>
+      <c r="F95">
+        <v>1145443573.60122</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_1_AutoML_3_20240527_104809_model_7</t>
+        </is>
+      </c>
+      <c r="B96">
+        <v>34539.5451536579</v>
+      </c>
+      <c r="C96">
+        <v>1192980179.42157</v>
+      </c>
+      <c r="D96">
+        <v>26069.8276926662</v>
+      </c>
+      <c r="F96">
+        <v>1192980179.42157</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_3_AutoML_3_20240527_104809_model_3</t>
+        </is>
+      </c>
+      <c r="B97">
+        <v>34818.5639274309</v>
+      </c>
+      <c r="C97">
+        <v>1212332393.96859</v>
+      </c>
+      <c r="D97">
+        <v>27219.7501105358</v>
+      </c>
+      <c r="E97">
+        <v>3.24055968571783</v>
+      </c>
+      <c r="F97">
+        <v>1212332393.96859</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>DeepLearning_1_AutoML_3_20240527_104809</t>
+        </is>
+      </c>
+      <c r="B98">
+        <v>34947.1502511154</v>
+      </c>
+      <c r="C98">
+        <v>1221303310.67403</v>
+      </c>
+      <c r="D98">
+        <v>25575.6275286154</v>
+      </c>
+      <c r="F98">
+        <v>1221303310.67403</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_1_AutoML_3_20240527_104809_model_2</t>
+        </is>
+      </c>
+      <c r="B99">
+        <v>35235.3167748404</v>
+      </c>
+      <c r="C99">
+        <v>1241527548.22335</v>
+      </c>
+      <c r="D99">
+        <v>26392.546385934</v>
+      </c>
+      <c r="F99">
+        <v>1241527548.22335</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_3_20240527_104809_model_144</t>
+        </is>
+      </c>
+      <c r="B100">
+        <v>38221.0257255814</v>
+      </c>
+      <c r="C100">
+        <v>1460846807.51556</v>
+      </c>
+      <c r="D100">
+        <v>30647.2060255287</v>
+      </c>
+      <c r="E100">
+        <v>3.3814873235953</v>
+      </c>
+      <c r="F100">
+        <v>1460846807.51556</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_2_AutoML_3_20240527_104809_model_2</t>
+        </is>
+      </c>
+      <c r="B101">
+        <v>38923.997199154</v>
+      </c>
+      <c r="C101">
+        <v>1515077557.95975</v>
+      </c>
+      <c r="D101">
+        <v>31798.6753453999</v>
+      </c>
+      <c r="E101">
+        <v>3.42007257975873</v>
+      </c>
+      <c r="F101">
+        <v>1515077557.95975</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_3_AutoML_3_20240527_104809_model_2</t>
+        </is>
+      </c>
+      <c r="B102">
+        <v>38938.6775841277</v>
+      </c>
+      <c r="C102">
+        <v>1516220612.00065</v>
+      </c>
+      <c r="D102">
+        <v>32428.7733129601</v>
+      </c>
+      <c r="E102">
+        <v>3.44033630782122</v>
+      </c>
+      <c r="F102">
+        <v>1516220612.00065</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_3_AutoML_3_20240527_104809_model_1</t>
+        </is>
+      </c>
+      <c r="B103">
+        <v>39426.6713121529</v>
+      </c>
+      <c r="C103">
+        <v>1554462410.75654</v>
+      </c>
+      <c r="D103">
+        <v>33868.6740842386</v>
+      </c>
+      <c r="E103">
+        <v>3.50183632128004</v>
+      </c>
+      <c r="F103">
+        <v>1554462410.75654</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_2_AutoML_3_20240527_104809_model_1</t>
+        </is>
+      </c>
+      <c r="B104">
+        <v>40314.6213018729</v>
+      </c>
+      <c r="C104">
+        <v>1625268690.71343</v>
+      </c>
+      <c r="D104">
+        <v>34710.738525744</v>
+      </c>
+      <c r="E104">
+        <v>3.51847713384562</v>
+      </c>
+      <c r="F104">
+        <v>1625268690.71343</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>GLM_1_AutoML_3_20240527_104809</t>
+        </is>
+      </c>
+      <c r="B105">
+        <v>45471.2286705947</v>
+      </c>
+      <c r="C105">
+        <v>2067632636.81352</v>
+      </c>
+      <c r="D105">
+        <v>36843.2118435683</v>
+      </c>
+      <c r="E105">
+        <v>3.48607621336647</v>
+      </c>
+      <c r="F105">
+        <v>2067632636.81352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor visualization code for wage prediction
</commit_message>
<xml_diff>
--- a/3.Applied-Supervised-Learning-Groupwork/trained_ML_models.xlsx
+++ b/3.Applied-Supervised-Learning-Groupwork/trained_ML_models.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -392,1462 +392,2056 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_2_AutoML_4_20240527_142625</t>
+          <t>StackedEnsemble_AllModels_6_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B2">
-        <v>26139.0539126436</v>
+        <v>25964.9013746912</v>
       </c>
       <c r="C2">
-        <v>683250139.448089</v>
+        <v>674176103.397439</v>
       </c>
       <c r="D2">
-        <v>18107.7455046202</v>
+        <v>18009.4816267214</v>
       </c>
       <c r="F2">
-        <v>683250139.448089</v>
+        <v>674176103.397439</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>StackedEnsemble_AllModels_1_AutoML_4_20240527_142625</t>
+          <t>StackedEnsemble_AllModels_5_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B3">
-        <v>26195.5107694089</v>
+        <v>25967.9060562725</v>
       </c>
       <c r="C3">
-        <v>686204784.470216</v>
+        <v>674332144.947392</v>
       </c>
       <c r="D3">
-        <v>18135.0393528394</v>
+        <v>17846.6097758543</v>
+      </c>
+      <c r="E3">
+        <v>2.95638233462593</v>
       </c>
       <c r="F3">
-        <v>686204784.470216</v>
+        <v>674332144.947392</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_2_AutoML_4_20240527_142625</t>
+          <t>StackedEnsemble_Best1000_1_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B4">
-        <v>26446.6304012854</v>
+        <v>25973.2885161127</v>
       </c>
       <c r="C4">
-        <v>699424259.582193</v>
+        <v>674611716.341233</v>
       </c>
       <c r="D4">
-        <v>18376.0625647871</v>
+        <v>18009.8252066791</v>
       </c>
       <c r="F4">
-        <v>699424259.582193</v>
+        <v>674611716.341233</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_3_AutoML_4_20240527_142625</t>
+          <t>StackedEnsemble_AllModels_3_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B5">
-        <v>26447.7592112792</v>
+        <v>25975.7267172851</v>
       </c>
       <c r="C5">
-        <v>699483967.297804</v>
+        <v>674738378.491079</v>
       </c>
       <c r="D5">
-        <v>18375.2250871511</v>
+        <v>18018.1599808612</v>
       </c>
       <c r="F5">
-        <v>699483967.297804</v>
+        <v>674738378.491079</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GBM_2_AutoML_4_20240527_142625</t>
+          <t>StackedEnsemble_AllModels_4_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B6">
-        <v>26448.6847880018</v>
+        <v>25977.457281805</v>
       </c>
       <c r="C6">
-        <v>699532927.01508</v>
+        <v>674828286.828006</v>
       </c>
       <c r="D6">
-        <v>18424.6251172095</v>
+        <v>18011.6860480138</v>
       </c>
       <c r="F6">
-        <v>699532927.01508</v>
+        <v>674828286.828006</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_50</t>
+          <t>StackedEnsemble_AllModels_2_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B7">
-        <v>26497.9481578339</v>
+        <v>26139.0539126436</v>
       </c>
       <c r="C7">
-        <v>702141256.575251</v>
+        <v>683250139.448089</v>
       </c>
       <c r="D7">
-        <v>18430.5243888819</v>
+        <v>18107.7455046202</v>
       </c>
       <c r="F7">
-        <v>702141256.575251</v>
+        <v>683250139.448089</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_40</t>
+          <t>StackedEnsemble_AllModels_1_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B8">
-        <v>26528.2635503011</v>
+        <v>26195.5107694089</v>
       </c>
       <c r="C8">
-        <v>703748766.994235</v>
+        <v>686204784.470216</v>
       </c>
       <c r="D8">
-        <v>18568.5033949879</v>
+        <v>18135.0393528394</v>
       </c>
       <c r="F8">
-        <v>703748766.994235</v>
+        <v>686204784.470216</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GBM_3_AutoML_4_20240527_142625</t>
+          <t>StackedEnsemble_BestOfFamily_4_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B9">
-        <v>26566.2077443975</v>
+        <v>26445.1230487547</v>
       </c>
       <c r="C9">
-        <v>705763393.918488</v>
+        <v>699344533.063778</v>
       </c>
       <c r="D9">
-        <v>18516.349918185</v>
+        <v>18373.1510775453</v>
       </c>
       <c r="F9">
-        <v>705763393.918488</v>
+        <v>699344533.063778</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GBM_5_AutoML_4_20240527_142625</t>
+          <t>StackedEnsemble_BestOfFamily_2_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B10">
-        <v>26635.2381552266</v>
+        <v>26446.6304012854</v>
       </c>
       <c r="C10">
-        <v>709435911.585636</v>
+        <v>699424259.582193</v>
       </c>
       <c r="D10">
-        <v>18638.0825366145</v>
+        <v>18376.0625647871</v>
       </c>
       <c r="F10">
-        <v>709435911.585636</v>
+        <v>699424259.582193</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_2</t>
+          <t>StackedEnsemble_BestOfFamily_3_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B11">
-        <v>26635.9521925523</v>
+        <v>26447.7592112792</v>
       </c>
       <c r="C11">
-        <v>709473949.203933</v>
+        <v>699483967.297804</v>
       </c>
       <c r="D11">
-        <v>18566.2289817685</v>
+        <v>18375.2250871511</v>
       </c>
       <c r="F11">
-        <v>709473949.203933</v>
+        <v>699483967.297804</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_11</t>
+          <t>GBM_2_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B12">
-        <v>26646.819587869</v>
+        <v>26448.6847880018</v>
       </c>
       <c r="C12">
-        <v>710052994.14844</v>
+        <v>699532927.01508</v>
       </c>
       <c r="D12">
-        <v>18595.7805973152</v>
+        <v>18424.6251172095</v>
       </c>
       <c r="F12">
-        <v>710052994.14844</v>
+        <v>699532927.01508</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_16</t>
+          <t>StackedEnsemble_BestOfFamily_6_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B13">
-        <v>26681.8595604156</v>
+        <v>26449.4568428324</v>
       </c>
       <c r="C13">
-        <v>711921629.6017441</v>
+        <v>699573767.280856</v>
       </c>
       <c r="D13">
-        <v>18879.9128485333</v>
+        <v>18385.7294774587</v>
       </c>
       <c r="F13">
-        <v>711921629.6017441</v>
+        <v>699573767.280856</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_54</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_50</t>
         </is>
       </c>
       <c r="B14">
-        <v>26718.9351713573</v>
+        <v>26497.9481578339</v>
       </c>
       <c r="C14">
-        <v>713901496.6911941</v>
+        <v>702141256.575251</v>
       </c>
       <c r="D14">
-        <v>18758.0875770022</v>
+        <v>18430.5243888819</v>
       </c>
       <c r="F14">
-        <v>713901496.6911941</v>
+        <v>702141256.575251</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_1</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_40</t>
         </is>
       </c>
       <c r="B15">
-        <v>26751.8348594465</v>
+        <v>26528.2635503011</v>
       </c>
       <c r="C15">
-        <v>715660668.347095</v>
+        <v>703748766.994235</v>
       </c>
       <c r="D15">
-        <v>18893.1045520578</v>
+        <v>18568.5033949879</v>
       </c>
       <c r="F15">
-        <v>715660668.347095</v>
+        <v>703748766.994235</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_13</t>
+          <t>GBM_3_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B16">
-        <v>26759.0645238962</v>
+        <v>26566.2077443975</v>
       </c>
       <c r="C16">
-        <v>716047534.1940399</v>
+        <v>705763393.918488</v>
       </c>
       <c r="D16">
-        <v>18759.5919927039</v>
+        <v>18516.349918185</v>
       </c>
       <c r="F16">
-        <v>716047534.1940399</v>
+        <v>705763393.918488</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_17</t>
+          <t>GBM_5_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B17">
-        <v>26792.1338909229</v>
+        <v>26635.2381552266</v>
       </c>
       <c r="C17">
-        <v>717818438.429137</v>
+        <v>709435911.585636</v>
       </c>
       <c r="D17">
-        <v>18816.0197141674</v>
+        <v>18638.0825366145</v>
       </c>
       <c r="F17">
-        <v>717818438.429137</v>
+        <v>709435911.585636</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_14</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_2</t>
         </is>
       </c>
       <c r="B18">
-        <v>26902.4248598273</v>
+        <v>26635.9521925523</v>
       </c>
       <c r="C18">
-        <v>723740463.3386559</v>
+        <v>709473949.203933</v>
       </c>
       <c r="D18">
-        <v>19017.389143322</v>
+        <v>18566.2289817685</v>
       </c>
       <c r="F18">
-        <v>723740463.3386559</v>
+        <v>709473949.203933</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_4</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_11</t>
         </is>
       </c>
       <c r="B19">
-        <v>26919.7291259043</v>
+        <v>26646.819587869</v>
       </c>
       <c r="C19">
-        <v>724671816.212063</v>
+        <v>710052994.14844</v>
       </c>
       <c r="D19">
-        <v>18955.0313269183</v>
+        <v>18595.7805973152</v>
       </c>
       <c r="F19">
-        <v>724671816.212063</v>
+        <v>710052994.14844</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_24</t>
+          <t>StackedEnsemble_BestOfFamily_5_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B20">
-        <v>26932.7932984761</v>
+        <v>26654.6819199843</v>
       </c>
       <c r="C20">
-        <v>725375354.858438</v>
+        <v>710472068.255538</v>
       </c>
       <c r="D20">
-        <v>18828.1444311479</v>
+        <v>18418.7458718058</v>
+      </c>
+      <c r="E20">
+        <v>2.96752696003754</v>
       </c>
       <c r="F20">
-        <v>725375354.858438</v>
+        <v>710472068.255538</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_5</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_16</t>
         </is>
       </c>
       <c r="B21">
-        <v>26949.6451511743</v>
+        <v>26681.8595604156</v>
       </c>
       <c r="C21">
-        <v>726283373.774215</v>
+        <v>711921629.6017441</v>
       </c>
       <c r="D21">
-        <v>18879.6434438751</v>
+        <v>18879.9128485333</v>
       </c>
       <c r="F21">
-        <v>726283373.774215</v>
+        <v>711921629.6017441</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_7</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_54</t>
         </is>
       </c>
       <c r="B22">
-        <v>26968.3315413661</v>
+        <v>26718.9351713573</v>
       </c>
       <c r="C22">
-        <v>727290906.125043</v>
+        <v>713901496.6911941</v>
       </c>
       <c r="D22">
-        <v>18958.861590561</v>
+        <v>18758.0875770022</v>
       </c>
       <c r="F22">
-        <v>727290906.125043</v>
+        <v>713901496.6911941</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_47</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_66</t>
         </is>
       </c>
       <c r="B23">
-        <v>26988.9752349013</v>
+        <v>26733.1255085381</v>
       </c>
       <c r="C23">
-        <v>728404784.230116</v>
+        <v>714659999.455253</v>
       </c>
       <c r="D23">
-        <v>19043.5406554007</v>
+        <v>18807.1078602155</v>
       </c>
       <c r="F23">
-        <v>728404784.230116</v>
+        <v>714659999.455253</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GBM_4_AutoML_4_20240527_142625</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_1</t>
         </is>
       </c>
       <c r="B24">
-        <v>27009.5972794545</v>
+        <v>26751.8348594465</v>
       </c>
       <c r="C24">
-        <v>729518345.198313</v>
+        <v>715660668.347095</v>
       </c>
       <c r="D24">
-        <v>18917.8452566798</v>
+        <v>18893.1045520578</v>
       </c>
       <c r="F24">
-        <v>729518345.198313</v>
+        <v>715660668.347095</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_20</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_13</t>
         </is>
       </c>
       <c r="B25">
-        <v>27014.6316056646</v>
+        <v>26759.0645238962</v>
       </c>
       <c r="C25">
-        <v>729790320.789775</v>
+        <v>716047534.1940399</v>
       </c>
       <c r="D25">
-        <v>19184.5637520741</v>
+        <v>18759.5919927039</v>
       </c>
       <c r="F25">
-        <v>729790320.789775</v>
+        <v>716047534.1940399</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_8</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_71</t>
         </is>
       </c>
       <c r="B26">
-        <v>27030.650949518</v>
+        <v>26761.1266089222</v>
       </c>
       <c r="C26">
-        <v>730656090.754676</v>
+        <v>716157897.3787659</v>
       </c>
       <c r="D26">
-        <v>18840.8898473663</v>
+        <v>18678.2676288795</v>
       </c>
       <c r="F26">
-        <v>730656090.754676</v>
+        <v>716157897.3787659</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_6</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_67</t>
         </is>
       </c>
       <c r="B27">
-        <v>27034.5406810572</v>
+        <v>26784.9948340399</v>
       </c>
       <c r="C27">
-        <v>730866389.835735</v>
+        <v>717435948.259546</v>
       </c>
       <c r="D27">
-        <v>18972.9566349748</v>
+        <v>18701.5843091421</v>
       </c>
       <c r="F27">
-        <v>730866389.835735</v>
+        <v>717435948.259546</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_27</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_17</t>
         </is>
       </c>
       <c r="B28">
-        <v>27053.8772873156</v>
+        <v>26792.1338909229</v>
       </c>
       <c r="C28">
-        <v>731912276.2771291</v>
+        <v>717818438.429137</v>
       </c>
       <c r="D28">
-        <v>19124.6560640986</v>
+        <v>18816.0197141674</v>
       </c>
       <c r="F28">
-        <v>731912276.2771291</v>
+        <v>717818438.429137</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_32</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_14</t>
         </is>
       </c>
       <c r="B29">
-        <v>27124.7776196183</v>
+        <v>26902.4248598273</v>
       </c>
       <c r="C29">
-        <v>735753560.913748</v>
+        <v>723740463.3386559</v>
       </c>
       <c r="D29">
-        <v>18982.0206388183</v>
+        <v>19017.389143322</v>
       </c>
       <c r="F29">
-        <v>735753560.913748</v>
+        <v>723740463.3386559</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_22</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_4</t>
         </is>
       </c>
       <c r="B30">
-        <v>27158.9178829692</v>
+        <v>26919.7291259043</v>
       </c>
       <c r="C30">
-        <v>737606820.573864</v>
+        <v>724671816.212063</v>
       </c>
       <c r="D30">
-        <v>19320.2249906561</v>
+        <v>18955.0313269183</v>
       </c>
       <c r="F30">
-        <v>737606820.573864</v>
+        <v>724671816.212063</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_44</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_24</t>
         </is>
       </c>
       <c r="B31">
-        <v>27169.7109973133</v>
+        <v>26932.7932984761</v>
       </c>
       <c r="C31">
-        <v>738193195.677527</v>
+        <v>725375354.858438</v>
       </c>
       <c r="D31">
-        <v>19061.1283260652</v>
+        <v>18828.1444311479</v>
       </c>
       <c r="F31">
-        <v>738193195.677527</v>
+        <v>725375354.858438</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_15</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_5</t>
         </is>
       </c>
       <c r="B32">
-        <v>27174.2149397502</v>
+        <v>26949.6451511743</v>
       </c>
       <c r="C32">
-        <v>738437957.591743</v>
+        <v>726283373.774215</v>
       </c>
       <c r="D32">
-        <v>19362.2641369533</v>
+        <v>18879.6434438751</v>
       </c>
       <c r="F32">
-        <v>738437957.591743</v>
+        <v>726283373.774215</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_46</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_7</t>
         </is>
       </c>
       <c r="B33">
-        <v>27174.8135234335</v>
+        <v>26968.3315413661</v>
       </c>
       <c r="C33">
-        <v>738470490.033385</v>
+        <v>727290906.125043</v>
       </c>
       <c r="D33">
-        <v>19052.1837858502</v>
+        <v>18958.861590561</v>
       </c>
       <c r="F33">
-        <v>738470490.033385</v>
+        <v>727290906.125043</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_48</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_47</t>
         </is>
       </c>
       <c r="B34">
-        <v>27214.0911365117</v>
+        <v>26988.9752349013</v>
       </c>
       <c r="C34">
-        <v>740606756.386363</v>
+        <v>728404784.230116</v>
       </c>
       <c r="D34">
-        <v>19216.9485521179</v>
+        <v>19043.5406554007</v>
       </c>
       <c r="F34">
-        <v>740606756.386363</v>
+        <v>728404784.230116</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_59</t>
+          <t>GBM_4_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B35">
-        <v>27292.7198854241</v>
+        <v>27009.5972794545</v>
       </c>
       <c r="C35">
-        <v>744892558.744223</v>
+        <v>729518345.198313</v>
       </c>
       <c r="D35">
-        <v>19088.576578518</v>
+        <v>18917.8452566798</v>
       </c>
       <c r="F35">
-        <v>744892558.744223</v>
+        <v>729518345.198313</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_35</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_20</t>
         </is>
       </c>
       <c r="B36">
-        <v>27293.082224832</v>
+        <v>27014.6316056646</v>
       </c>
       <c r="C36">
-        <v>744912337.331439</v>
+        <v>729790320.789775</v>
       </c>
       <c r="D36">
-        <v>19347.5793313203</v>
+        <v>19184.5637520741</v>
       </c>
       <c r="F36">
-        <v>744912337.331439</v>
+        <v>729790320.789775</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_58</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_8</t>
         </is>
       </c>
       <c r="B37">
-        <v>27370.6080902144</v>
+        <v>27030.650949518</v>
       </c>
       <c r="C37">
-        <v>749150187.228109</v>
+        <v>730656090.754676</v>
       </c>
       <c r="D37">
-        <v>19318.8395531854</v>
+        <v>18840.8898473663</v>
       </c>
       <c r="F37">
-        <v>749150187.228109</v>
+        <v>730656090.754676</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_41</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_6</t>
         </is>
       </c>
       <c r="B38">
-        <v>27427.2518774566</v>
+        <v>27034.5406810572</v>
       </c>
       <c r="C38">
-        <v>752254145.549444</v>
+        <v>730866389.835735</v>
       </c>
       <c r="D38">
-        <v>19486.7205030844</v>
+        <v>18972.9566349748</v>
       </c>
       <c r="F38">
-        <v>752254145.549444</v>
+        <v>730866389.835735</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_30</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_27</t>
         </is>
       </c>
       <c r="B39">
-        <v>27439.7105372804</v>
+        <v>27053.8772873156</v>
       </c>
       <c r="C39">
-        <v>752937714.3697391</v>
+        <v>731912276.2771291</v>
       </c>
       <c r="D39">
-        <v>19134.9828389745</v>
+        <v>19124.6560640986</v>
       </c>
       <c r="F39">
-        <v>752937714.3697391</v>
+        <v>731912276.2771291</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_60</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_70</t>
         </is>
       </c>
       <c r="B40">
-        <v>27445.9876498188</v>
+        <v>27071.0460146</v>
       </c>
       <c r="C40">
-        <v>753282238.074006</v>
+        <v>732841532.324592</v>
       </c>
       <c r="D40">
-        <v>19335.4018074429</v>
+        <v>18934.2866406056</v>
       </c>
       <c r="F40">
-        <v>753282238.074006</v>
+        <v>732841532.324592</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>StackedEnsemble_BestOfFamily_1_AutoML_4_20240527_142625</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_32</t>
         </is>
       </c>
       <c r="B41">
-        <v>27457.0057155853</v>
+        <v>27124.7776196183</v>
       </c>
       <c r="C41">
-        <v>753887162.8656861</v>
+        <v>735753560.913748</v>
       </c>
       <c r="D41">
-        <v>19153.6787885979</v>
+        <v>18982.0206388183</v>
       </c>
       <c r="F41">
-        <v>753887162.8656861</v>
+        <v>735753560.913748</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>GBM_1_AutoML_4_20240527_142625</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_22</t>
         </is>
       </c>
       <c r="B42">
-        <v>27462.2819525765</v>
+        <v>27158.9178829692</v>
       </c>
       <c r="C42">
-        <v>754176930.04281</v>
+        <v>737606820.573864</v>
       </c>
       <c r="D42">
-        <v>19183.2736384172</v>
+        <v>19320.2249906561</v>
       </c>
       <c r="F42">
-        <v>754176930.04281</v>
+        <v>737606820.573864</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_45</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_44</t>
         </is>
       </c>
       <c r="B43">
-        <v>27562.4461922221</v>
+        <v>27169.7109973133</v>
       </c>
       <c r="C43">
-        <v>759688440.099141</v>
+        <v>738193195.677527</v>
       </c>
       <c r="D43">
-        <v>19321.6619767985</v>
+        <v>19061.1283260652</v>
       </c>
       <c r="F43">
-        <v>759688440.099141</v>
+        <v>738193195.677527</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_49</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_15</t>
         </is>
       </c>
       <c r="B44">
-        <v>27637.5748985135</v>
+        <v>27174.2149397502</v>
       </c>
       <c r="C44">
-        <v>763835546.270945</v>
+        <v>738437957.591743</v>
       </c>
       <c r="D44">
-        <v>19681.1039691576</v>
+        <v>19362.2641369533</v>
       </c>
       <c r="F44">
-        <v>763835546.270945</v>
+        <v>738437957.591743</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_10</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_46</t>
         </is>
       </c>
       <c r="B45">
-        <v>27689.9821676463</v>
+        <v>27174.8135234335</v>
       </c>
       <c r="C45">
-        <v>766735112.444572</v>
+        <v>738470490.033385</v>
       </c>
       <c r="D45">
-        <v>19439.0977918421</v>
+        <v>19052.1837858502</v>
       </c>
       <c r="F45">
-        <v>766735112.444572</v>
+        <v>738470490.033385</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_34</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_48</t>
         </is>
       </c>
       <c r="B46">
-        <v>27691.5180768571</v>
+        <v>27214.0911365117</v>
       </c>
       <c r="C46">
-        <v>766820173.400905</v>
+        <v>740606756.386363</v>
       </c>
       <c r="D46">
-        <v>19345.9171915572</v>
+        <v>19216.9485521179</v>
       </c>
       <c r="F46">
-        <v>766820173.400905</v>
+        <v>740606756.386363</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_19</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_59</t>
         </is>
       </c>
       <c r="B47">
-        <v>27741.6994411372</v>
+        <v>27292.7198854241</v>
       </c>
       <c r="C47">
-        <v>769601887.882395</v>
+        <v>744892558.744223</v>
       </c>
       <c r="D47">
-        <v>19611.8932864877</v>
+        <v>19088.576578518</v>
       </c>
       <c r="F47">
-        <v>769601887.882395</v>
+        <v>744892558.744223</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_25</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_35</t>
         </is>
       </c>
       <c r="B48">
-        <v>27747.8546991663</v>
+        <v>27293.082224832</v>
       </c>
       <c r="C48">
-        <v>769943440.4060481</v>
+        <v>744912337.331439</v>
       </c>
       <c r="D48">
-        <v>19722.0070910669</v>
+        <v>19347.5793313203</v>
       </c>
       <c r="F48">
-        <v>769943440.4060481</v>
+        <v>744912337.331439</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_26</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_58</t>
         </is>
       </c>
       <c r="B49">
-        <v>27784.490668406</v>
+        <v>27370.6080902144</v>
       </c>
       <c r="C49">
-        <v>771977921.702742</v>
+        <v>749150187.228109</v>
       </c>
       <c r="D49">
-        <v>19681.6939316651</v>
+        <v>19318.8395531854</v>
       </c>
       <c r="F49">
-        <v>771977921.702742</v>
+        <v>749150187.228109</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_55</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_41</t>
         </is>
       </c>
       <c r="B50">
-        <v>27796.1043776928</v>
+        <v>27427.2518774566</v>
       </c>
       <c r="C50">
-        <v>772623418.575596</v>
+        <v>752254145.549444</v>
       </c>
       <c r="D50">
-        <v>19580.6031428312</v>
+        <v>19486.7205030844</v>
       </c>
       <c r="F50">
-        <v>772623418.575596</v>
+        <v>752254145.549444</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_39</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_30</t>
         </is>
       </c>
       <c r="B51">
-        <v>27817.7507239784</v>
+        <v>27439.7105372804</v>
       </c>
       <c r="C51">
-        <v>773827255.341399</v>
+        <v>752937714.3697391</v>
       </c>
       <c r="D51">
-        <v>19692.3765594083</v>
+        <v>19134.9828389745</v>
       </c>
       <c r="F51">
-        <v>773827255.341399</v>
+        <v>752937714.3697391</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_53</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_60</t>
         </is>
       </c>
       <c r="B52">
-        <v>27849.587481715</v>
+        <v>27445.9876498188</v>
       </c>
       <c r="C52">
-        <v>775599522.9016941</v>
+        <v>753282238.074006</v>
       </c>
       <c r="D52">
-        <v>19549.6206862723</v>
+        <v>19335.4018074429</v>
       </c>
       <c r="F52">
-        <v>775599522.9016941</v>
+        <v>753282238.074006</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_21</t>
+          <t>StackedEnsemble_BestOfFamily_1_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B53">
-        <v>27890.8163397751</v>
+        <v>27457.0057155853</v>
       </c>
       <c r="C53">
-        <v>777897636.099064</v>
+        <v>753887162.8656861</v>
       </c>
       <c r="D53">
-        <v>19993.7378265136</v>
+        <v>19153.6787885979</v>
       </c>
       <c r="F53">
-        <v>777897636.099064</v>
+        <v>753887162.8656861</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_3</t>
+          <t>GBM_1_AutoML_5_20240527_161714</t>
         </is>
       </c>
       <c r="B54">
-        <v>27965.4314370224</v>
+        <v>27462.2819525765</v>
       </c>
       <c r="C54">
-        <v>782065355.4588</v>
+        <v>754176930.04281</v>
       </c>
       <c r="D54">
-        <v>19762.7450208328</v>
+        <v>19183.2736384172</v>
       </c>
       <c r="F54">
-        <v>782065355.4588</v>
+        <v>754176930.04281</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_57</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_45</t>
         </is>
       </c>
       <c r="B55">
-        <v>27991.8476353481</v>
+        <v>27562.4461922221</v>
       </c>
       <c r="C55">
-        <v>783543534.0405411</v>
+        <v>759688440.099141</v>
       </c>
       <c r="D55">
-        <v>19840.182130707</v>
+        <v>19321.6619767985</v>
       </c>
       <c r="F55">
-        <v>783543534.0405411</v>
+        <v>759688440.099141</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_56</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_49</t>
         </is>
       </c>
       <c r="B56">
-        <v>27993.5021887644</v>
+        <v>27637.5748985135</v>
       </c>
       <c r="C56">
-        <v>783636164.792357</v>
+        <v>763835546.270945</v>
       </c>
       <c r="D56">
-        <v>19697.5143610761</v>
+        <v>19681.1039691576</v>
       </c>
       <c r="F56">
-        <v>783636164.792357</v>
+        <v>763835546.270945</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_51</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_10</t>
         </is>
       </c>
       <c r="B57">
-        <v>27998.4568371644</v>
+        <v>27689.9821676463</v>
       </c>
       <c r="C57">
-        <v>783913585.262561</v>
+        <v>766735112.444572</v>
       </c>
       <c r="D57">
-        <v>19745.1488225765</v>
+        <v>19439.0977918421</v>
       </c>
       <c r="F57">
-        <v>783913585.262561</v>
+        <v>766735112.444572</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_52</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_34</t>
         </is>
       </c>
       <c r="B58">
-        <v>28006.4164081842</v>
+        <v>27691.5180768571</v>
       </c>
       <c r="C58">
-        <v>784359360.028607</v>
+        <v>766820173.400905</v>
       </c>
       <c r="D58">
-        <v>19823.2587798588</v>
+        <v>19345.9171915572</v>
       </c>
       <c r="F58">
-        <v>784359360.028607</v>
+        <v>766820173.400905</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_33</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_19</t>
         </is>
       </c>
       <c r="B59">
-        <v>28011.8174424215</v>
+        <v>27741.6994411372</v>
       </c>
       <c r="C59">
-        <v>784661916.427551</v>
+        <v>769601887.882395</v>
       </c>
       <c r="D59">
-        <v>20111.6065573157</v>
+        <v>19611.8932864877</v>
       </c>
       <c r="F59">
-        <v>784661916.427551</v>
+        <v>769601887.882395</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_37</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_25</t>
         </is>
       </c>
       <c r="B60">
-        <v>28023.6027793018</v>
+        <v>27747.8546991663</v>
       </c>
       <c r="C60">
-        <v>785322312.732094</v>
+        <v>769943440.4060481</v>
       </c>
       <c r="D60">
-        <v>19730.6686503769</v>
+        <v>19722.0070910669</v>
       </c>
       <c r="F60">
-        <v>785322312.732094</v>
+        <v>769943440.4060481</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_36</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_65</t>
         </is>
       </c>
       <c r="B61">
-        <v>28046.1899987905</v>
+        <v>27760.542322574</v>
       </c>
       <c r="C61">
-        <v>786588773.448256</v>
+        <v>770647710.0434231</v>
       </c>
       <c r="D61">
-        <v>19991.2930852843</v>
+        <v>19813.2575891327</v>
       </c>
       <c r="F61">
-        <v>786588773.448256</v>
+        <v>770647710.0434231</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_43</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_26</t>
         </is>
       </c>
       <c r="B62">
-        <v>28087.2745351917</v>
+        <v>27784.490668406</v>
       </c>
       <c r="C62">
-        <v>788894990.815227</v>
+        <v>771977921.702742</v>
       </c>
       <c r="D62">
-        <v>19894.308260214</v>
+        <v>19681.6939316651</v>
       </c>
       <c r="F62">
-        <v>788894990.815227</v>
+        <v>771977921.702742</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_38</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_55</t>
         </is>
       </c>
       <c r="B63">
-        <v>28092.8297127636</v>
+        <v>27796.1043776928</v>
       </c>
       <c r="C63">
-        <v>789207081.270336</v>
+        <v>772623418.575596</v>
       </c>
       <c r="D63">
-        <v>19835.0800003641</v>
+        <v>19580.6031428312</v>
       </c>
       <c r="F63">
-        <v>789207081.270336</v>
+        <v>772623418.575596</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_42</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_39</t>
         </is>
       </c>
       <c r="B64">
-        <v>28199.9986289864</v>
+        <v>27817.7507239784</v>
       </c>
       <c r="C64">
-        <v>795239922.674835</v>
+        <v>773827255.341399</v>
       </c>
       <c r="D64">
-        <v>20278.1753332654</v>
+        <v>19692.3765594083</v>
       </c>
       <c r="F64">
-        <v>795239922.674835</v>
+        <v>773827255.341399</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_61</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_53</t>
         </is>
       </c>
       <c r="B65">
-        <v>28227.5315432764</v>
+        <v>27849.587481715</v>
       </c>
       <c r="C65">
-        <v>796793537.026662</v>
+        <v>775599522.9016941</v>
       </c>
       <c r="D65">
-        <v>19984.3956550779</v>
+        <v>19549.6206862723</v>
       </c>
       <c r="F65">
-        <v>796793537.026662</v>
+        <v>775599522.9016941</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_28</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_62</t>
         </is>
       </c>
       <c r="B66">
-        <v>28445.6945333818</v>
+        <v>27884.6492399808</v>
       </c>
       <c r="C66">
-        <v>809157537.486467</v>
+        <v>777553663.2367589</v>
       </c>
       <c r="D66">
-        <v>20625.0437320281</v>
+        <v>19725.1279113983</v>
       </c>
       <c r="F66">
-        <v>809157537.486467</v>
+        <v>777553663.2367589</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_23</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_21</t>
         </is>
       </c>
       <c r="B67">
-        <v>28512.4470335386</v>
+        <v>27890.8163397751</v>
       </c>
       <c r="C67">
-        <v>812959635.840345</v>
+        <v>777897636.099064</v>
       </c>
       <c r="D67">
-        <v>20497.9063902774</v>
+        <v>19993.7378265136</v>
       </c>
       <c r="F67">
-        <v>812959635.840345</v>
+        <v>777897636.099064</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_31</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_3</t>
         </is>
       </c>
       <c r="B68">
-        <v>28700.1194058359</v>
+        <v>27965.4314370224</v>
       </c>
       <c r="C68">
-        <v>823696853.909241</v>
+        <v>782065355.4588</v>
       </c>
       <c r="D68">
-        <v>20481.3610981412</v>
+        <v>19762.7450208328</v>
       </c>
       <c r="F68">
-        <v>823696853.909241</v>
+        <v>782065355.4588</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_9</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_57</t>
         </is>
       </c>
       <c r="B69">
-        <v>28994.6855035035</v>
+        <v>27991.8476353481</v>
       </c>
       <c r="C69">
-        <v>840691787.447075</v>
+        <v>783543534.0405411</v>
       </c>
       <c r="D69">
-        <v>20651.1665011592</v>
-      </c>
-      <c r="E69">
-        <v>2.99827664054663</v>
+        <v>19840.182130707</v>
       </c>
       <c r="F69">
-        <v>840691787.447075</v>
+        <v>783543534.0405411</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_29</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_56</t>
         </is>
       </c>
       <c r="B70">
-        <v>29053.9221738493</v>
+        <v>27993.5021887644</v>
       </c>
       <c r="C70">
-        <v>844130393.684094</v>
+        <v>783636164.792357</v>
       </c>
       <c r="D70">
-        <v>20767.0606671311</v>
+        <v>19697.5143610761</v>
       </c>
       <c r="F70">
-        <v>844130393.684094</v>
+        <v>783636164.792357</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>DRF_1_AutoML_4_20240527_142625</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_51</t>
         </is>
       </c>
       <c r="B71">
-        <v>29056.0297884051</v>
+        <v>27998.4568371644</v>
       </c>
       <c r="C71">
-        <v>844252867.064684</v>
+        <v>783913585.262561</v>
       </c>
       <c r="D71">
-        <v>20922.9173172925</v>
-      </c>
-      <c r="E71">
-        <v>3.02971297689165</v>
+        <v>19745.1488225765</v>
       </c>
       <c r="F71">
-        <v>844252867.064684</v>
+        <v>783913585.262561</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_18</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_52</t>
         </is>
       </c>
       <c r="B72">
-        <v>29106.1924671242</v>
+        <v>28006.4164081842</v>
       </c>
       <c r="C72">
-        <v>847170439.933277</v>
+        <v>784359360.028607</v>
       </c>
       <c r="D72">
-        <v>21239.1948189763</v>
+        <v>19823.2587798588</v>
       </c>
       <c r="F72">
-        <v>847170439.933277</v>
+        <v>784359360.028607</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>XRT_1_AutoML_4_20240527_142625</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_33</t>
         </is>
       </c>
       <c r="B73">
-        <v>29280.5830655129</v>
+        <v>28011.8174424215</v>
       </c>
       <c r="C73">
-        <v>857352544.656399</v>
+        <v>784661916.427551</v>
       </c>
       <c r="D73">
-        <v>21311.8507868639</v>
-      </c>
-      <c r="E73">
-        <v>3.05415933953721</v>
+        <v>20111.6065573157</v>
       </c>
       <c r="F73">
-        <v>857352544.656399</v>
+        <v>784661916.427551</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_12</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_37</t>
         </is>
       </c>
       <c r="B74">
-        <v>29385.9002333859</v>
+        <v>28023.6027793018</v>
       </c>
       <c r="C74">
-        <v>863531132.52651</v>
+        <v>785322312.732094</v>
       </c>
       <c r="D74">
-        <v>21413.4247674038</v>
-      </c>
-      <c r="E74">
-        <v>3.04216380190729</v>
+        <v>19730.6686503769</v>
       </c>
       <c r="F74">
-        <v>863531132.52651</v>
+        <v>785322312.732094</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>DeepLearning_1_AutoML_4_20240527_142625</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_36</t>
         </is>
       </c>
       <c r="B75">
-        <v>34644.5925091591</v>
+        <v>28046.1899987905</v>
       </c>
       <c r="C75">
-        <v>1200247790.12568</v>
+        <v>786588773.448256</v>
       </c>
       <c r="D75">
-        <v>25629.1528714276</v>
+        <v>19991.2930852843</v>
       </c>
       <c r="F75">
-        <v>1200247790.12568</v>
+        <v>786588773.448256</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>GBM_grid_1_AutoML_4_20240527_142625_model_62</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_43</t>
         </is>
       </c>
       <c r="B76">
-        <v>34653.4185097706</v>
+        <v>28087.2745351917</v>
       </c>
       <c r="C76">
-        <v>1200859414.41331</v>
+        <v>788894990.815227</v>
       </c>
       <c r="D76">
-        <v>27368.0099334208</v>
-      </c>
-      <c r="E76">
-        <v>3.32011275175191</v>
+        <v>19894.308260214</v>
       </c>
       <c r="F76">
-        <v>1200859414.41331</v>
+        <v>788894990.815227</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>GLM_1_AutoML_4_20240527_142625</t>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_38</t>
         </is>
       </c>
       <c r="B77">
+        <v>28092.8297127636</v>
+      </c>
+      <c r="C77">
+        <v>789207081.270336</v>
+      </c>
+      <c r="D77">
+        <v>19835.0800003641</v>
+      </c>
+      <c r="F77">
+        <v>789207081.270336</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_61</t>
+        </is>
+      </c>
+      <c r="B78">
+        <v>28165.4299087612</v>
+      </c>
+      <c r="C78">
+        <v>793291441.94534</v>
+      </c>
+      <c r="D78">
+        <v>19892.0732550875</v>
+      </c>
+      <c r="F78">
+        <v>793291441.94534</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_42</t>
+        </is>
+      </c>
+      <c r="B79">
+        <v>28199.9986289864</v>
+      </c>
+      <c r="C79">
+        <v>795239922.674835</v>
+      </c>
+      <c r="D79">
+        <v>20278.1753332654</v>
+      </c>
+      <c r="F79">
+        <v>795239922.674835</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_63</t>
+        </is>
+      </c>
+      <c r="B80">
+        <v>28228.0915732443</v>
+      </c>
+      <c r="C80">
+        <v>796825153.867466</v>
+      </c>
+      <c r="D80">
+        <v>19929.8103838264</v>
+      </c>
+      <c r="F80">
+        <v>796825153.867466</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_68</t>
+        </is>
+      </c>
+      <c r="B81">
+        <v>28258.1641667075</v>
+      </c>
+      <c r="C81">
+        <v>798523842.072593</v>
+      </c>
+      <c r="D81">
+        <v>20221.3325488025</v>
+      </c>
+      <c r="F81">
+        <v>798523842.072593</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_64</t>
+        </is>
+      </c>
+      <c r="B82">
+        <v>28271.9971908048</v>
+      </c>
+      <c r="C82">
+        <v>799305825.156872</v>
+      </c>
+      <c r="D82">
+        <v>20055.3046436175</v>
+      </c>
+      <c r="F82">
+        <v>799305825.156872</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_69</t>
+        </is>
+      </c>
+      <c r="B83">
+        <v>28275.5970841074</v>
+      </c>
+      <c r="C83">
+        <v>799509390.462783</v>
+      </c>
+      <c r="D83">
+        <v>20102.8909330691</v>
+      </c>
+      <c r="F83">
+        <v>799509390.462783</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_28</t>
+        </is>
+      </c>
+      <c r="B84">
+        <v>28445.6945333818</v>
+      </c>
+      <c r="C84">
+        <v>809157537.486467</v>
+      </c>
+      <c r="D84">
+        <v>20625.0437320281</v>
+      </c>
+      <c r="F84">
+        <v>809157537.486467</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_23</t>
+        </is>
+      </c>
+      <c r="B85">
+        <v>28512.4470335386</v>
+      </c>
+      <c r="C85">
+        <v>812959635.840345</v>
+      </c>
+      <c r="D85">
+        <v>20497.9063902774</v>
+      </c>
+      <c r="F85">
+        <v>812959635.840345</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_143</t>
+        </is>
+      </c>
+      <c r="B86">
+        <v>28513.8269784476</v>
+      </c>
+      <c r="C86">
+        <v>813038328.956847</v>
+      </c>
+      <c r="D86">
+        <v>20552.0235027454</v>
+      </c>
+      <c r="F86">
+        <v>813038328.956847</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_31</t>
+        </is>
+      </c>
+      <c r="B87">
+        <v>28700.1194058359</v>
+      </c>
+      <c r="C87">
+        <v>823696853.909241</v>
+      </c>
+      <c r="D87">
+        <v>20481.3610981412</v>
+      </c>
+      <c r="F87">
+        <v>823696853.909241</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_9</t>
+        </is>
+      </c>
+      <c r="B88">
+        <v>28994.6855035035</v>
+      </c>
+      <c r="C88">
+        <v>840691787.447075</v>
+      </c>
+      <c r="D88">
+        <v>20651.1665011592</v>
+      </c>
+      <c r="E88">
+        <v>2.99827664054663</v>
+      </c>
+      <c r="F88">
+        <v>840691787.447075</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_29</t>
+        </is>
+      </c>
+      <c r="B89">
+        <v>29053.9221738493</v>
+      </c>
+      <c r="C89">
+        <v>844130393.684094</v>
+      </c>
+      <c r="D89">
+        <v>20767.0606671311</v>
+      </c>
+      <c r="F89">
+        <v>844130393.684094</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>DRF_1_AutoML_5_20240527_161714</t>
+        </is>
+      </c>
+      <c r="B90">
+        <v>29056.0297884051</v>
+      </c>
+      <c r="C90">
+        <v>844252867.064684</v>
+      </c>
+      <c r="D90">
+        <v>20922.9173172925</v>
+      </c>
+      <c r="E90">
+        <v>3.02971297689165</v>
+      </c>
+      <c r="F90">
+        <v>844252867.064684</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_18</t>
+        </is>
+      </c>
+      <c r="B91">
+        <v>29106.1924671242</v>
+      </c>
+      <c r="C91">
+        <v>847170439.933277</v>
+      </c>
+      <c r="D91">
+        <v>21239.1948189763</v>
+      </c>
+      <c r="F91">
+        <v>847170439.933277</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>XRT_1_AutoML_5_20240527_161714</t>
+        </is>
+      </c>
+      <c r="B92">
+        <v>29280.5830655129</v>
+      </c>
+      <c r="C92">
+        <v>857352544.656399</v>
+      </c>
+      <c r="D92">
+        <v>21311.8507868639</v>
+      </c>
+      <c r="E92">
+        <v>3.05415933953721</v>
+      </c>
+      <c r="F92">
+        <v>857352544.656399</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_12</t>
+        </is>
+      </c>
+      <c r="B93">
+        <v>29385.9002333859</v>
+      </c>
+      <c r="C93">
+        <v>863531132.52651</v>
+      </c>
+      <c r="D93">
+        <v>21413.4247674038</v>
+      </c>
+      <c r="E93">
+        <v>3.04216380190729</v>
+      </c>
+      <c r="F93">
+        <v>863531132.52651</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_1_AutoML_5_20240527_161714_model_3</t>
+        </is>
+      </c>
+      <c r="B94">
+        <v>33427.6850722061</v>
+      </c>
+      <c r="C94">
+        <v>1117410129.28659</v>
+      </c>
+      <c r="D94">
+        <v>25013.8199122343</v>
+      </c>
+      <c r="F94">
+        <v>1117410129.28659</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_1_AutoML_5_20240527_161714_model_1</t>
+        </is>
+      </c>
+      <c r="B95">
+        <v>33657.0665363296</v>
+      </c>
+      <c r="C95">
+        <v>1132798127.83091</v>
+      </c>
+      <c r="D95">
+        <v>25047.8618011365</v>
+      </c>
+      <c r="F95">
+        <v>1132798127.83091</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_2_AutoML_5_20240527_161714_model_3</t>
+        </is>
+      </c>
+      <c r="B96">
+        <v>34492.9640309286</v>
+      </c>
+      <c r="C96">
+        <v>1189764567.63893</v>
+      </c>
+      <c r="D96">
+        <v>26819.9311971803</v>
+      </c>
+      <c r="E96">
+        <v>3.2338922481091</v>
+      </c>
+      <c r="F96">
+        <v>1189764567.63893</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_3_AutoML_5_20240527_161714_model_3</t>
+        </is>
+      </c>
+      <c r="B97">
+        <v>34648.2755308748</v>
+      </c>
+      <c r="C97">
+        <v>1200502997.26342</v>
+      </c>
+      <c r="D97">
+        <v>26824.1162107522</v>
+      </c>
+      <c r="E97">
+        <v>3.22253405527066</v>
+      </c>
+      <c r="F97">
+        <v>1200502997.26342</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>DeepLearning_1_AutoML_5_20240527_161714</t>
+        </is>
+      </c>
+      <c r="B98">
+        <v>35252.5197759152</v>
+      </c>
+      <c r="C98">
+        <v>1242740150.55129</v>
+      </c>
+      <c r="D98">
+        <v>25555.217418626</v>
+      </c>
+      <c r="F98">
+        <v>1242740150.55129</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_1_AutoML_5_20240527_161714_model_4</t>
+        </is>
+      </c>
+      <c r="B99">
+        <v>35290.7589996558</v>
+      </c>
+      <c r="C99">
+        <v>1245437670.77179</v>
+      </c>
+      <c r="D99">
+        <v>27046.790955113</v>
+      </c>
+      <c r="F99">
+        <v>1245437670.77179</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_1_AutoML_5_20240527_161714_model_2</t>
+        </is>
+      </c>
+      <c r="B100">
+        <v>35482.6794282687</v>
+      </c>
+      <c r="C100">
+        <v>1259020539.40928</v>
+      </c>
+      <c r="D100">
+        <v>26454.9819911932</v>
+      </c>
+      <c r="F100">
+        <v>1259020539.40928</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_3_AutoML_5_20240527_161714_model_1</t>
+        </is>
+      </c>
+      <c r="B101">
+        <v>37665.880458858</v>
+      </c>
+      <c r="C101">
+        <v>1418718550.74098</v>
+      </c>
+      <c r="D101">
+        <v>32022.4086066773</v>
+      </c>
+      <c r="E101">
+        <v>3.46668235521475</v>
+      </c>
+      <c r="F101">
+        <v>1418718550.74098</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_1_AutoML_5_20240527_161714_model_9</t>
+        </is>
+      </c>
+      <c r="B102">
+        <v>37830.8635891324</v>
+      </c>
+      <c r="C102">
+        <v>1431174239.89955</v>
+      </c>
+      <c r="D102">
+        <v>29277.7534642947</v>
+      </c>
+      <c r="F102">
+        <v>1431174239.89955</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_2_AutoML_5_20240527_161714_model_2</t>
+        </is>
+      </c>
+      <c r="B103">
+        <v>39043.5371760139</v>
+      </c>
+      <c r="C103">
+        <v>1524397795.21478</v>
+      </c>
+      <c r="D103">
+        <v>31430.5295205695</v>
+      </c>
+      <c r="E103">
+        <v>3.39866652918025</v>
+      </c>
+      <c r="F103">
+        <v>1524397795.21478</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>GBM_grid_1_AutoML_5_20240527_161714_model_144</t>
+        </is>
+      </c>
+      <c r="B104">
+        <v>39294.1666415823</v>
+      </c>
+      <c r="C104">
+        <v>1544031532.05644</v>
+      </c>
+      <c r="D104">
+        <v>31595.2621878798</v>
+      </c>
+      <c r="E104">
+        <v>3.39927542173016</v>
+      </c>
+      <c r="F104">
+        <v>1544031532.05644</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_2_AutoML_5_20240527_161714_model_1</t>
+        </is>
+      </c>
+      <c r="B105">
+        <v>39302.540601943</v>
+      </c>
+      <c r="C105">
+        <v>1544689697.76738</v>
+      </c>
+      <c r="D105">
+        <v>33462.0184616535</v>
+      </c>
+      <c r="E105">
+        <v>3.4952898153759</v>
+      </c>
+      <c r="F105">
+        <v>1544689697.76738</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>DeepLearning_grid_3_AutoML_5_20240527_161714_model_2</t>
+        </is>
+      </c>
+      <c r="B106">
+        <v>39730.651383695</v>
+      </c>
+      <c r="C106">
+        <v>1578524659.37271</v>
+      </c>
+      <c r="D106">
+        <v>31832.9548161752</v>
+      </c>
+      <c r="E106">
+        <v>3.39977899372691</v>
+      </c>
+      <c r="F106">
+        <v>1578524659.37271</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>GLM_1_AutoML_5_20240527_161714</t>
+        </is>
+      </c>
+      <c r="B107">
         <v>45471.2286705947</v>
       </c>
-      <c r="C77">
+      <c r="C107">
         <v>2067632636.81352</v>
       </c>
-      <c r="D77">
+      <c r="D107">
         <v>36843.2118435683</v>
       </c>
-      <c r="E77">
+      <c r="E107">
         <v>3.48607621336647</v>
       </c>
-      <c r="F77">
+      <c r="F107">
         <v>2067632636.81352</v>
       </c>
     </row>

</xml_diff>